<commit_message>
Change wording on number of cold boxes
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -843,12 +843,6 @@
     <t>Contact Phone Number</t>
   </si>
   <si>
-    <t>Number of cold boxes at facility</t>
-  </si>
-  <si>
-    <t>Number of vaccine carriers at facility</t>
-  </si>
-  <si>
     <t>Number of freeze safe cold boxes at facility</t>
   </si>
   <si>
@@ -882,30 +876,12 @@
     <t>Teléfono de contacto?</t>
   </si>
   <si>
-    <t>Number of cold boxes at facility?</t>
-  </si>
-  <si>
-    <t>Number of vaccine carriers at facility?</t>
-  </si>
-  <si>
     <t>Number of freeze safe cold boxes at facility?</t>
   </si>
   <si>
     <t>Number of freeze safe vaccine carriers at facility?</t>
   </si>
   <si>
-    <t>Número de cajas frías en la facilidad</t>
-  </si>
-  <si>
-    <t>Número de portadores de vacunas en la facilidad</t>
-  </si>
-  <si>
-    <t>Número de cajas frías en la facilidad?</t>
-  </si>
-  <si>
-    <t>Número de portadores de vacunas en la facilidad?</t>
-  </si>
-  <si>
     <t>Número de cajas frías a congelación segura en la facilidad</t>
   </si>
   <si>
@@ -1081,6 +1057,30 @@
   </si>
   <si>
     <t>(kilómetros)</t>
+  </si>
+  <si>
+    <t>Total number of cold boxes at facility</t>
+  </si>
+  <si>
+    <t>Total number of vaccine carriers at facility</t>
+  </si>
+  <si>
+    <t>Número total de cajas frías en la facilidad</t>
+  </si>
+  <si>
+    <t>Número total de portadores de vacunas en la facilidad</t>
+  </si>
+  <si>
+    <t>Total number of cold boxes at facility?</t>
+  </si>
+  <si>
+    <t>Número total de cajas frías en la facilidad?</t>
+  </si>
+  <si>
+    <t>Total number of vaccine carriers at facility?</t>
+  </si>
+  <si>
+    <t>Número total de portadores de vacunas en la facilidad?</t>
   </si>
 </sst>
 </file>
@@ -1639,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1649,7 +1649,7 @@
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.58203125" customWidth="1"/>
     <col min="6" max="6" width="43.25" customWidth="1"/>
     <col min="7" max="8" width="26.83203125" customWidth="1"/>
     <col min="9" max="12" width="47.6640625" customWidth="1"/>
@@ -1685,10 +1685,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -1800,10 +1800,10 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E8" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -1882,19 +1882,19 @@
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="F13" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G13" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H13" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="I13" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -1935,7 +1935,7 @@
         <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1961,10 +1961,10 @@
         <v>51</v>
       </c>
       <c r="J18" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="K18" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1977,19 +1977,19 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E20" t="s">
         <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G20" t="s">
         <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I20" t="s">
         <v>55</v>
@@ -2022,13 +2022,13 @@
         <v>61</v>
       </c>
       <c r="I23" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="J23" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="K23" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -2036,13 +2036,13 @@
         <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E24" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F24" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G24" t="s">
         <v>63</v>
@@ -2051,7 +2051,7 @@
         <v>64</v>
       </c>
       <c r="I24" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -2078,10 +2078,10 @@
         <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="I27" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -2104,7 +2104,7 @@
         <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -2134,7 +2134,7 @@
         <v>76</v>
       </c>
       <c r="I31" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -2148,13 +2148,13 @@
         <v>267</v>
       </c>
       <c r="G32" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="H32" t="s">
+        <v>277</v>
+      </c>
+      <c r="I32" s="10" t="s">
         <v>278</v>
-      </c>
-      <c r="H32" t="s">
-        <v>279</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
@@ -2170,13 +2170,13 @@
         <v>269</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H33" t="s">
         <v>269</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
@@ -2196,19 +2196,19 @@
         <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F36" t="s">
-        <v>270</v>
+        <v>342</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>287</v>
+        <v>344</v>
       </c>
       <c r="H36" t="s">
-        <v>283</v>
+        <v>346</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>289</v>
+        <v>347</v>
       </c>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
@@ -2218,19 +2218,19 @@
         <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H37" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I37" s="12" t="s">
         <v>284</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>290</v>
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -2252,19 +2252,19 @@
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>272</v>
+        <v>343</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>285</v>
+        <v>348</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>292</v>
+        <v>349</v>
       </c>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
@@ -2274,19 +2274,19 @@
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H41" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="I41" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>294</v>
       </c>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -2511,13 +2511,13 @@
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C15" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
@@ -2553,13 +2553,13 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D18" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -2651,13 +2651,13 @@
         <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C27" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D27" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -2679,7 +2679,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C29" t="s">
         <v>141</v>
@@ -2693,13 +2693,13 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C30" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D30" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -2707,13 +2707,13 @@
         <v>42</v>
       </c>
       <c r="B31" t="s">
+        <v>310</v>
+      </c>
+      <c r="C31" t="s">
         <v>318</v>
       </c>
-      <c r="C31" t="s">
-        <v>326</v>
-      </c>
       <c r="D31" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -2802,7 +2802,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B40" t="s">
         <v>159</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s">
         <v>162</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B42" t="s">
         <v>164</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B43" t="s">
         <v>167</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B44" t="s">
         <v>170</v>
@@ -2956,21 +2956,21 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B54" t="s">
         <v>189</v>
       </c>
       <c r="C54" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D54" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B55" t="s">
         <v>190</v>
@@ -2984,10 +2984,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s">
         <v>193</v>
@@ -2998,21 +2998,21 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B57" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C57" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D57" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B58" t="s">
         <v>143</v>
@@ -3195,22 +3195,22 @@
     </row>
     <row r="3" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
         <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -3277,7 +3277,7 @@
         <v>225</v>
       </c>
       <c r="B2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -3285,10 +3285,10 @@
         <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="D4" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -3296,7 +3296,7 @@
         <v>227</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
@@ -3420,7 +3420,7 @@
         <v>243</v>
       </c>
       <c r="E3" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3437,7 +3437,7 @@
         <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3454,7 +3454,7 @@
         <v>243</v>
       </c>
       <c r="E5" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update with latest french translations
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500"/>
+    <workbookView xWindow="2500" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,11 @@
     <sheet name="properties" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="441">
   <si>
     <t>clause</t>
   </si>
@@ -1081,6 +1073,279 @@
   </si>
   <si>
     <t>Número total de portadores de vacunas en la facilidad?</t>
+  </si>
+  <si>
+    <t>display.title.text.fr</t>
+  </si>
+  <si>
+    <t>display.prompt.text.fr</t>
+  </si>
+  <si>
+    <t>display.hint.text.fr</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Entrepôt national de vaccins</t>
+  </si>
+  <si>
+    <t>Entrepôt régional de vaccins</t>
+  </si>
+  <si>
+    <t>Entrepôt de vaccins de district</t>
+  </si>
+  <si>
+    <t>Hôpital central</t>
+  </si>
+  <si>
+    <t>Hôpital de district</t>
+  </si>
+  <si>
+    <t>Hôpital rural</t>
+  </si>
+  <si>
+    <t>Hôpital</t>
+  </si>
+  <si>
+    <t>Hôpital communautaire</t>
+  </si>
+  <si>
+    <t>Centre de santé</t>
+  </si>
+  <si>
+    <t>Dispensaire</t>
+  </si>
+  <si>
+    <t>Station de santé</t>
+  </si>
+  <si>
+    <t>Poste de santé</t>
+  </si>
+  <si>
+    <t>Maternité</t>
+  </si>
+  <si>
+    <t>Privé</t>
+  </si>
+  <si>
+    <t>Confessionnel</t>
+  </si>
+  <si>
+    <t>Autre</t>
+  </si>
+  <si>
+    <t>Électricité</t>
+  </si>
+  <si>
+    <t>Énergie solaire</t>
+  </si>
+  <si>
+    <t>Groupe électrogène</t>
+  </si>
+  <si>
+    <t>Électricité et groupe électrogène</t>
+  </si>
+  <si>
+    <t>Électricité et énergie solaire</t>
+  </si>
+  <si>
+    <t>Groupe électrogène et énergie solaire</t>
+  </si>
+  <si>
+    <t>Aucune source d'énergie</t>
+  </si>
+  <si>
+    <t>Plus de 16</t>
+  </si>
+  <si>
+    <t>8 à 16</t>
+  </si>
+  <si>
+    <t>4 à 8</t>
+  </si>
+  <si>
+    <t>Moins de 4</t>
+  </si>
+  <si>
+    <t>Aucun</t>
+  </si>
+  <si>
+    <t>Disponible de façon irrégulière</t>
+  </si>
+  <si>
+    <t>Non disponible</t>
+  </si>
+  <si>
+    <t>Ne sais pas</t>
+  </si>
+  <si>
+    <t>Sans objet</t>
+  </si>
+  <si>
+    <t>Modéré</t>
+  </si>
+  <si>
+    <t>Tempéré</t>
+  </si>
+  <si>
+    <t>Chaud</t>
+  </si>
+  <si>
+    <t>Dépôt</t>
+  </si>
+  <si>
+    <t>Livraison</t>
+  </si>
+  <si>
+    <t>Dépôt et livraison</t>
+  </si>
+  <si>
+    <t>Poste fixe</t>
+  </si>
+  <si>
+    <t>Ambulant</t>
+  </si>
+  <si>
+    <t>Fixe et ambulant</t>
+  </si>
+  <si>
+    <t>Stockage uniquement</t>
+  </si>
+  <si>
+    <t>Livré</t>
+  </si>
+  <si>
+    <t>Collecté</t>
+  </si>
+  <si>
+    <t>Livré et collecté</t>
+  </si>
+  <si>
+    <t>Nom de l'établissement</t>
+  </si>
+  <si>
+    <t>ID de l'établissement</t>
+  </si>
+  <si>
+    <t>Localisation</t>
+  </si>
+  <si>
+    <t>Région administrative</t>
+  </si>
+  <si>
+    <t>Type d'établissement</t>
+  </si>
+  <si>
+    <t>Propriétaire de l'établissement</t>
+  </si>
+  <si>
+    <t>Population desservie</t>
+  </si>
+  <si>
+    <t>Source d'électricité</t>
+  </si>
+  <si>
+    <t>Électricité disponible</t>
+  </si>
+  <si>
+    <t>Carburant disponible</t>
+  </si>
+  <si>
+    <t>Distance par rapport au lieu d'approvisionnement le plus proche</t>
+  </si>
+  <si>
+    <t>Services de vaccination proposés</t>
+  </si>
+  <si>
+    <t>Intervalle entre chaque approvisionnement</t>
+  </si>
+  <si>
+    <t>Mode d'approvisionnement</t>
+  </si>
+  <si>
+    <t>Nom de la personne à contacter</t>
+  </si>
+  <si>
+    <t>Titre de la personne à contacter</t>
+  </si>
+  <si>
+    <t>Numéro de téléphone de la personne à contacter</t>
+  </si>
+  <si>
+    <t>Nombre de glacières dans l'établissement</t>
+  </si>
+  <si>
+    <t>Nombre de porte-vaccins dans l'établissement</t>
+  </si>
+  <si>
+    <t>Nombre de glacières pour congélation sûre dans l'établissement</t>
+  </si>
+  <si>
+    <t>Nombre de porte-vaccins pour congélation sûre dans l'établissement</t>
+  </si>
+  <si>
+    <t>Entrer le nom de l'établissement de santé</t>
+  </si>
+  <si>
+    <t>Entrer l'ID de l'établissement de santé</t>
+  </si>
+  <si>
+    <t>Choisir le type d'établissement</t>
+  </si>
+  <si>
+    <t>Choisir le propriétaire</t>
+  </si>
+  <si>
+    <t>Entrer la population desservie</t>
+  </si>
+  <si>
+    <t>Choisir la source d'électricité</t>
+  </si>
+  <si>
+    <t>Indiquer si l'électricité est disponible</t>
+  </si>
+  <si>
+    <t>Indiquer si le carburant est disponible</t>
+  </si>
+  <si>
+    <t>À quelle distance se trouve le lieu d'approvisionnement le plus proche ?</t>
+  </si>
+  <si>
+    <t>Mode de livraison</t>
+  </si>
+  <si>
+    <t>Intervalle (nombre de semaines) entre chaque approvisionnement en vaccins</t>
+  </si>
+  <si>
+    <t>Mode d'approvisionnement en vaccins</t>
+  </si>
+  <si>
+    <t>Établissement de santé</t>
+  </si>
+  <si>
+    <t>display.locale.text.fr</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>Espagnol</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Francés</t>
+  </si>
+  <si>
+    <t>Français</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1458,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1224,6 +1489,39 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1637,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="G29" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1650,13 +1948,14 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="35.58203125" customWidth="1"/>
-    <col min="6" max="6" width="43.25" customWidth="1"/>
-    <col min="7" max="8" width="26.83203125" customWidth="1"/>
-    <col min="9" max="12" width="47.6640625" customWidth="1"/>
-    <col min="13" max="1027" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
+    <col min="8" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="15" width="47.6640625" customWidth="1"/>
+    <col min="16" max="1030" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1678,26 +1977,35 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1706,14 +2014,17 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1727,21 +2038,28 @@
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="23" t="s">
+        <v>421</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="1" t="b">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -1754,28 +2072,38 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" t="b">
+      <c r="K4" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="P4" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H5" s="17"/>
+      <c r="K5" s="22"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H6" s="17"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -1788,14 +2116,20 @@
       <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K7" s="24" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>26</v>
       </c>
@@ -1811,27 +2145,37 @@
       <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="M8">
+      <c r="K8" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="P8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H9" s="17"/>
+      <c r="K9" s="22"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H10" s="17"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>29</v>
       </c>
@@ -1847,14 +2191,20 @@
       <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K11" s="24" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>29</v>
       </c>
@@ -1870,14 +2220,20 @@
       <c r="G12" t="s">
         <v>38</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="I12" t="s">
         <v>39</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K12" s="24" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>40</v>
       </c>
@@ -1890,24 +2246,34 @@
       <c r="G13" t="s">
         <v>289</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="I13" t="s">
         <v>290</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K13" s="24" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H14" s="17"/>
+      <c r="K14" s="22"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H15" s="17"/>
+      <c r="K15" s="22"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>29</v>
       </c>
@@ -1923,22 +2289,30 @@
       <c r="G16" t="s">
         <v>45</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="I16" t="s">
         <v>46</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K16" s="24" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H17" s="17"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>29</v>
       </c>
@@ -1954,25 +2328,33 @@
       <c r="G18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="I18" t="s">
         <v>52</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>51</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="L18" t="s">
         <v>338</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H19" s="17"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>29</v>
       </c>
@@ -1988,24 +2370,34 @@
       <c r="G20" t="s">
         <v>55</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="I20" t="s">
         <v>295</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K20" s="25" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H21" s="17"/>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H22" s="17"/>
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>41</v>
       </c>
@@ -2018,20 +2410,26 @@
       <c r="G23" t="s">
         <v>60</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="I23" t="s">
         <v>61</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>301</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="L23" t="s">
         <v>340</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>29</v>
       </c>
@@ -2047,24 +2445,34 @@
       <c r="G24" t="s">
         <v>63</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="I24" t="s">
         <v>64</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K24" s="24" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H25" s="17"/>
+      <c r="K25" s="22"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H26" s="17"/>
+      <c r="K26" s="22"/>
+    </row>
+    <row r="27" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>40</v>
       </c>
@@ -2077,14 +2485,20 @@
       <c r="G27" t="s">
         <v>67</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="I27" t="s">
         <v>296</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K27" s="25" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>29</v>
       </c>
@@ -2100,24 +2514,34 @@
       <c r="G28" t="s">
         <v>71</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="I28" t="s">
         <v>72</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K28" s="25" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H29" s="17"/>
+      <c r="K29" s="22"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H30" s="17"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>12</v>
       </c>
@@ -2130,14 +2554,20 @@
       <c r="G31" t="s">
         <v>75</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="I31" t="s">
         <v>76</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K31" s="25" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>12</v>
       </c>
@@ -2150,16 +2580,23 @@
       <c r="G32" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="I32" t="s">
         <v>277</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="J32" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K32" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+    </row>
+    <row r="33" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>12</v>
       </c>
@@ -2172,26 +2609,37 @@
       <c r="G33" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="I33" t="s">
         <v>269</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="J33" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K33" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H34" s="17"/>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="17"/>
+      <c r="K35" s="22"/>
+    </row>
+    <row r="36" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" t="s">
         <v>40</v>
       </c>
@@ -2204,16 +2652,23 @@
       <c r="G36" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="I36" t="s">
         <v>346</v>
       </c>
-      <c r="I36" s="11" t="s">
+      <c r="J36" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-    </row>
-    <row r="37" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K36" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+    </row>
+    <row r="37" spans="1:14" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C37" t="s">
         <v>40</v>
       </c>
@@ -2226,28 +2681,39 @@
       <c r="G37" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="J37" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-    </row>
-    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K37" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+    </row>
+    <row r="38" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H38" s="17"/>
+      <c r="K38" s="22"/>
+    </row>
+    <row r="39" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H39" s="17"/>
+      <c r="K39" s="22"/>
+    </row>
+    <row r="40" spans="1:14" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C40" t="s">
         <v>40</v>
       </c>
@@ -2260,16 +2726,23 @@
       <c r="G40" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="I40" s="12" t="s">
+      <c r="J40" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K40" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:14" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C41" t="s">
         <v>40</v>
       </c>
@@ -2282,37 +2755,41 @@
       <c r="G41" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H41" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="I41" s="12" t="s">
+      <c r="J41" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K41" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>21</v>
       </c>
+      <c r="H42" s="17"/>
+      <c r="K42" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2320,11 +2797,12 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="1025" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="30.58203125" customWidth="1"/>
+    <col min="5" max="5" width="29.08203125" customWidth="1"/>
+    <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -2337,8 +2815,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -2351,8 +2832,11 @@
       <c r="D2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2365,8 +2849,11 @@
       <c r="D3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2379,8 +2866,11 @@
       <c r="D5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="15" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2393,8 +2883,11 @@
       <c r="D6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2407,8 +2900,11 @@
       <c r="D7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2421,8 +2917,11 @@
       <c r="D8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2435,8 +2934,11 @@
       <c r="D9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="15" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2449,8 +2951,11 @@
       <c r="D10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -2463,8 +2968,11 @@
       <c r="D11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" s="15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2477,8 +2985,11 @@
       <c r="D12" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" s="15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2491,8 +3002,11 @@
       <c r="D13" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="15" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2505,8 +3019,11 @@
       <c r="D14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" s="15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2519,8 +3036,11 @@
       <c r="D15" s="11" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="15" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2533,8 +3053,11 @@
       <c r="D16" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2547,8 +3070,11 @@
       <c r="D17" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="15" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2562,7 +3088,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2575,8 +3101,11 @@
       <c r="D20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2589,8 +3118,11 @@
       <c r="D21" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" s="15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2603,8 +3135,11 @@
       <c r="D22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2617,8 +3152,11 @@
       <c r="D23" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" s="15" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2631,8 +3169,11 @@
       <c r="D24" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" s="15" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2645,8 +3186,11 @@
       <c r="D26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" s="15" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2659,8 +3203,11 @@
       <c r="D27" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" s="15" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2673,8 +3220,11 @@
       <c r="D28" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" s="15" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2687,8 +3237,11 @@
       <c r="D29" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="16" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2701,8 +3254,11 @@
       <c r="D30" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2715,8 +3271,11 @@
       <c r="D31" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="16" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2729,8 +3288,11 @@
       <c r="D32" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="15" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2743,8 +3305,11 @@
       <c r="D34" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" s="15" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2757,8 +3322,11 @@
       <c r="D35" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" s="15" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2771,8 +3339,11 @@
       <c r="D36" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" s="15" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2785,8 +3356,11 @@
       <c r="D37" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" s="15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2799,8 +3373,11 @@
       <c r="D38" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38" s="15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>293</v>
       </c>
@@ -2813,8 +3390,11 @@
       <c r="D40" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>293</v>
       </c>
@@ -2827,8 +3407,11 @@
       <c r="D41" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41" s="15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>293</v>
       </c>
@@ -2841,8 +3424,11 @@
       <c r="D42" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42" s="15" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>293</v>
       </c>
@@ -2855,8 +3441,11 @@
       <c r="D43" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43" s="15" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>293</v>
       </c>
@@ -2869,8 +3458,11 @@
       <c r="D44" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44" s="15" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2883,8 +3475,11 @@
       <c r="D46" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46" s="15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -2897,8 +3492,11 @@
       <c r="D47" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47" s="15" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -2911,8 +3509,11 @@
       <c r="D48" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48" s="15" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -2925,8 +3526,11 @@
       <c r="D50" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50" s="15" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2939,8 +3543,11 @@
       <c r="D51" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" s="15" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -2953,8 +3560,11 @@
       <c r="D52" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" s="15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>292</v>
       </c>
@@ -2967,8 +3577,11 @@
       <c r="D54" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>292</v>
       </c>
@@ -2981,8 +3594,11 @@
       <c r="D55" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" s="15" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>292</v>
       </c>
@@ -2995,8 +3611,11 @@
       <c r="D56" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" s="15" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>292</v>
       </c>
@@ -3009,8 +3628,11 @@
       <c r="D57" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" s="15" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>292</v>
       </c>
@@ -3023,8 +3645,11 @@
       <c r="D58" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E58" s="15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -3037,8 +3662,11 @@
       <c r="D60" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" s="15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3051,8 +3679,11 @@
       <c r="D61" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" s="15" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3065,8 +3696,11 @@
       <c r="D62" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E62" s="16" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -3079,8 +3713,11 @@
       <c r="D63" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" s="15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -3092,16 +3729,14 @@
       </c>
       <c r="D64" t="s">
         <v>169</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3238,21 +3873,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+    <col min="4" max="4" width="18.4140625" customWidth="1"/>
+    <col min="5" max="5" width="18.4140625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.9140625" customWidth="1"/>
+    <col min="8" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -3265,22 +3904,30 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" t="s">
         <v>223</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="30" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>225</v>
       </c>
       <c r="B2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E2" s="27"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -3290,16 +3937,22 @@
       <c r="D4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E4" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>227</v>
       </c>
       <c r="B5" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="E5" s="27"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>228</v>
       </c>
@@ -3307,53 +3960,76 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="27"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>229</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="27"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>230</v>
       </c>
       <c r="B8" s="7">
         <v>20170807</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="27"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>231</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" t="s">
         <v>232</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H9" s="30" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>234</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="27"/>
+      <c r="F10" t="s">
         <v>235</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>236</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>437</v>
+      </c>
+      <c r="F11" t="s">
+        <v>438</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Sort admin regions by regionName
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2505" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="489">
   <si>
     <t>clause</t>
   </si>
@@ -1485,6 +1485,12 @@
   </si>
   <si>
     <t>sub_district_vaccine_store</t>
+  </si>
+  <si>
+    <t>order_by</t>
+  </si>
+  <si>
+    <t>regionName</t>
   </si>
 </sst>
 </file>
@@ -1602,7 +1608,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1668,6 +1674,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2088,7 +2097,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" style="29" customWidth="1"/>
     <col min="2" max="2" width="8.75" style="29"/>
@@ -2118,7 +2127,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5">
+    <row r="3" spans="1:4" ht="78.75">
       <c r="A3" s="1" t="s">
         <v>444</v>
       </c>
@@ -2138,21 +2147,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView topLeftCell="G29" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.58203125" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="35.625" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
-    <col min="7" max="7" width="33.83203125" customWidth="1"/>
-    <col min="8" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="15" width="47.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.875" customWidth="1"/>
+    <col min="8" max="9" width="26.875" customWidth="1"/>
+    <col min="10" max="15" width="47.625" customWidth="1"/>
     <col min="16" max="1030" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2225,7 +2234,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="25" customHeight="1">
+    <row r="3" spans="1:16" ht="24.95" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2598,7 +2607,7 @@
       <c r="H22" s="17"/>
       <c r="K22" s="22"/>
     </row>
-    <row r="23" spans="1:14" ht="46.5">
+    <row r="23" spans="1:14" ht="47.25">
       <c r="C23" t="s">
         <v>41</v>
       </c>
@@ -2673,7 +2682,7 @@
       <c r="H26" s="17"/>
       <c r="K26" s="22"/>
     </row>
-    <row r="27" spans="1:14" ht="31">
+    <row r="27" spans="1:14" ht="31.5">
       <c r="C27" t="s">
         <v>40</v>
       </c>
@@ -2742,7 +2751,7 @@
       <c r="H30" s="17"/>
       <c r="K30" s="22"/>
     </row>
-    <row r="31" spans="1:14" ht="31">
+    <row r="31" spans="1:14" ht="31.5">
       <c r="C31" t="s">
         <v>12</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="31">
+    <row r="32" spans="1:14" ht="31.5">
       <c r="C32" t="s">
         <v>12</v>
       </c>
@@ -2797,7 +2806,7 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
     </row>
-    <row r="33" spans="1:14" ht="31">
+    <row r="33" spans="1:14" ht="31.5">
       <c r="C33" t="s">
         <v>12</v>
       </c>
@@ -2840,7 +2849,7 @@
       <c r="H35" s="17"/>
       <c r="K35" s="22"/>
     </row>
-    <row r="36" spans="1:14" ht="31.5" thickBot="1">
+    <row r="36" spans="1:14" ht="32.25" thickBot="1">
       <c r="C36" t="s">
         <v>40</v>
       </c>
@@ -2869,7 +2878,7 @@
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
     </row>
-    <row r="37" spans="1:14" ht="44" thickBot="1">
+    <row r="37" spans="1:14" ht="45.75" thickBot="1">
       <c r="C37" t="s">
         <v>40</v>
       </c>
@@ -2898,7 +2907,7 @@
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
     </row>
-    <row r="38" spans="1:14" ht="16" thickBot="1">
+    <row r="38" spans="1:14" ht="16.5" thickBot="1">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -2906,7 +2915,7 @@
       <c r="H38" s="17"/>
       <c r="K38" s="22"/>
     </row>
-    <row r="39" spans="1:14" ht="16" thickBot="1">
+    <row r="39" spans="1:14" ht="16.5" thickBot="1">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2914,7 +2923,7 @@
       <c r="H39" s="17"/>
       <c r="K39" s="22"/>
     </row>
-    <row r="40" spans="1:14" ht="29.5" thickBot="1">
+    <row r="40" spans="1:14" ht="30.75" thickBot="1">
       <c r="C40" t="s">
         <v>40</v>
       </c>
@@ -2943,7 +2952,7 @@
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
     </row>
-    <row r="41" spans="1:14" ht="44" thickBot="1">
+    <row r="41" spans="1:14" ht="45.75" thickBot="1">
       <c r="C41" t="s">
         <v>40</v>
       </c>
@@ -2989,21 +2998,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.58203125" customWidth="1"/>
-    <col min="5" max="5" width="29.08203125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="30.625" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
     <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17" customHeight="1">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17" customHeight="1">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3653,7 +3662,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="31">
+    <row r="45" spans="1:5" ht="31.5">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -4137,29 +4146,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="57.6640625" customWidth="1"/>
-    <col min="10" max="10" width="43.1640625" customWidth="1"/>
-    <col min="11" max="11" width="35.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.875" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="7" max="7" width="25.625" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="9" max="9" width="23.375" customWidth="1"/>
+    <col min="10" max="10" width="43.125" customWidth="1"/>
+    <col min="11" max="11" width="35.125" customWidth="1"/>
     <col min="12" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1">
+    <row r="1" spans="1:12" ht="21" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>203</v>
       </c>
@@ -4193,8 +4202,11 @@
       <c r="K1" s="5" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="26" customHeight="1">
+      <c r="L1" s="32" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="26.1" customHeight="1">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -4223,7 +4235,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45.75" customHeight="1">
+    <row r="3" spans="1:12" ht="45.75" customHeight="1">
       <c r="A3" t="s">
         <v>329</v>
       </c>
@@ -4251,8 +4263,11 @@
       <c r="K3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="64.75" customHeight="1">
+      <c r="L3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="64.7" customHeight="1">
       <c r="I4" s="1"/>
     </row>
   </sheetData>
@@ -4274,15 +4289,15 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="18.4140625" customWidth="1"/>
-    <col min="5" max="5" width="18.4140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.9140625" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="18.375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="18.875" customWidth="1"/>
     <col min="8" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4347,7 +4362,7 @@
       <c r="E5" s="27"/>
       <c r="H5" s="29"/>
     </row>
-    <row r="6" spans="1:8" ht="31">
+    <row r="6" spans="1:8" ht="31.5">
       <c r="A6" s="6" t="s">
         <v>228</v>
       </c>
@@ -4436,10 +4451,10 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Ask user explicitly before allowing move to a different facility
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2510" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
     <sheet name="survey" sheetId="1" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" r:id="rId3"/>
-    <sheet name="queries" sheetId="3" r:id="rId4"/>
-    <sheet name="settings" sheetId="4" r:id="rId5"/>
-    <sheet name="properties" sheetId="5" r:id="rId6"/>
+    <sheet name="model" sheetId="7" r:id="rId3"/>
+    <sheet name="choices" sheetId="2" r:id="rId4"/>
+    <sheet name="queries" sheetId="3" r:id="rId5"/>
+    <sheet name="settings" sheetId="4" r:id="rId6"/>
+    <sheet name="properties" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="497">
   <si>
     <t>clause</t>
   </si>
@@ -1491,6 +1492,30 @@
   </si>
   <si>
     <t>regionName</t>
+  </si>
+  <si>
+    <t>isSessionVariable</t>
+  </si>
+  <si>
+    <t>change_admin_region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>Change Admin Region</t>
+  </si>
+  <si>
+    <t>Cambiar región administrativa</t>
+  </si>
+  <si>
+    <t>¿Desea mover esta facilidad a una región / distrito diferente?</t>
+  </si>
+  <si>
+    <t>Do you want to move this facility to a different region/district?</t>
+  </si>
+  <si>
+    <t>selected(data('change_admin_region'), 'yes')</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1586,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1572,6 +1597,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFABF8F"/>
         <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1608,7 +1639,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1678,6 +1709,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2097,7 +2129,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="16" style="29" customWidth="1"/>
     <col min="2" max="2" width="8.75" style="29"/>
@@ -2127,7 +2159,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="78.75">
+    <row r="3" spans="1:4" ht="77.5">
       <c r="A3" s="1" t="s">
         <v>444</v>
       </c>
@@ -2145,23 +2177,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="1" max="1" width="25.58203125" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="5" width="35.625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.58203125" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
-    <col min="7" max="7" width="33.875" customWidth="1"/>
-    <col min="8" max="9" width="26.875" customWidth="1"/>
-    <col min="10" max="15" width="47.625" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
+    <col min="8" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="15" width="47.58203125" customWidth="1"/>
     <col min="16" max="1030" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2234,7 +2266,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="24.95" customHeight="1">
+    <row r="3" spans="1:16" ht="25" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2339,654 +2371,694 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="C8" t="s">
+    <row r="8" spans="1:16" s="33" customFormat="1">
+      <c r="C8" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>490</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>495</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="29" customFormat="1">
+      <c r="A9" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>496</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>329</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>320</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H10" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" t="s">
         <v>27</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="P8">
+      <c r="P10">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
+    <row r="11" spans="1:16" s="29" customFormat="1">
+      <c r="A11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="K9" s="22"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
+      <c r="H12" s="17"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="K10" s="22"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="C11" t="s">
+      <c r="H13" s="17"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F14" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G14" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I14" t="s">
         <v>34</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J14" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K14" s="24" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="C12" t="s">
+    <row r="15" spans="1:16">
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F15" t="s">
         <v>37</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G15" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>405</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I15" t="s">
         <v>39</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J15" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K15" s="24" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>287</v>
-      </c>
-      <c r="F13" t="s">
-        <v>288</v>
-      </c>
-      <c r="G13" t="s">
-        <v>289</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="I13" t="s">
-        <v>290</v>
-      </c>
-      <c r="J13" t="s">
-        <v>289</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="17"/>
-      <c r="K14" s="22"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="17"/>
-      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:16">
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>287</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>288</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>290</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>289</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>337</v>
+        <v>21</v>
       </c>
       <c r="H17" s="17"/>
       <c r="K17" s="22"/>
     </row>
-    <row r="18" spans="1:14">
-      <c r="C18" t="s">
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
         <v>48</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E21" t="s">
         <v>49</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G21" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H21" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I21" t="s">
         <v>52</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J21" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="K21" s="25" t="s">
         <v>427</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L21" t="s">
         <v>338</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M21" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
         <v>53</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>293</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>294</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="I20" t="s">
-        <v>295</v>
-      </c>
-      <c r="J20" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" t="s">
-        <v>11</v>
       </c>
       <c r="H22" s="17"/>
       <c r="K22" s="22"/>
     </row>
-    <row r="23" spans="1:14" ht="47.25">
+    <row r="23" spans="1:13">
       <c r="C23" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>293</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>294</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>410</v>
+        <v>55</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>409</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>295</v>
       </c>
       <c r="J23" t="s">
-        <v>301</v>
+        <v>55</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="L23" t="s">
-        <v>340</v>
-      </c>
-      <c r="M23" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>292</v>
-      </c>
-      <c r="E24" t="s">
-        <v>331</v>
-      </c>
-      <c r="F24" t="s">
-        <v>291</v>
-      </c>
-      <c r="G24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="I24" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" t="s">
-        <v>297</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="K24" s="22"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="H25" s="17"/>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:14">
-      <c r="A26" t="s">
+    <row r="26" spans="1:13" ht="46.5">
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="I26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" t="s">
+        <v>301</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="L26" t="s">
+        <v>340</v>
+      </c>
+      <c r="M26" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>292</v>
+      </c>
+      <c r="E27" t="s">
+        <v>331</v>
+      </c>
+      <c r="F27" t="s">
+        <v>291</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="I27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" t="s">
+        <v>297</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="K28" s="22"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
         <v>11</v>
-      </c>
-      <c r="H26" s="17"/>
-      <c r="K26" s="22"/>
-    </row>
-    <row r="27" spans="1:14" ht="31.5">
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>412</v>
-      </c>
-      <c r="I27" t="s">
-        <v>296</v>
-      </c>
-      <c r="J27" t="s">
-        <v>298</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" t="s">
-        <v>71</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="I28" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" t="s">
-        <v>299</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" t="s">
-        <v>21</v>
       </c>
       <c r="H29" s="17"/>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" spans="1:14">
-      <c r="A30" t="s">
+    <row r="30" spans="1:13" ht="31">
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="I30" t="s">
+        <v>296</v>
+      </c>
+      <c r="J30" t="s">
+        <v>298</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" t="s">
+        <v>299</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="K32" s="22"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="17"/>
-      <c r="K30" s="22"/>
-    </row>
-    <row r="31" spans="1:14" ht="31.5">
-      <c r="C31" t="s">
+      <c r="H33" s="17"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:14" ht="31">
+      <c r="C34" t="s">
         <v>12</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
         <v>73</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F34" t="s">
         <v>74</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G34" t="s">
         <v>75</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H34" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I34" t="s">
         <v>76</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J34" t="s">
         <v>300</v>
       </c>
-      <c r="K31" s="25" t="s">
+      <c r="K34" s="25" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="31.5">
-      <c r="C32" t="s">
+    <row r="35" spans="1:14" ht="31">
+      <c r="C35" t="s">
         <v>12</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>266</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F35" t="s">
         <v>267</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H35" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I35" t="s">
         <v>277</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J35" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="K32" s="25" t="s">
+      <c r="K35" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-    </row>
-    <row r="33" spans="1:14" ht="31.5">
-      <c r="C33" t="s">
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+    </row>
+    <row r="36" spans="1:14" ht="31">
+      <c r="C36" t="s">
         <v>12</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E36" t="s">
         <v>268</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F36" t="s">
         <v>269</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G36" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H36" s="20" t="s">
         <v>416</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I36" t="s">
         <v>269</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J36" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K33" s="25" t="s">
+      <c r="K36" s="25" t="s">
         <v>416</v>
-      </c>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="17"/>
-      <c r="K34" s="22"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="17"/>
-      <c r="K35" s="22"/>
-    </row>
-    <row r="36" spans="1:14" ht="32.25" thickBot="1">
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" t="s">
-        <v>272</v>
-      </c>
-      <c r="F36" t="s">
-        <v>342</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>417</v>
-      </c>
-      <c r="I36" t="s">
-        <v>346</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="K36" s="25" t="s">
-        <v>417</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
     </row>
-    <row r="37" spans="1:14" ht="45.75" thickBot="1">
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" t="s">
-        <v>274</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="H37" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="K37" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-    </row>
-    <row r="38" spans="1:14" ht="16.5" thickBot="1">
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="17"/>
+      <c r="K37" s="22"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="9"/>
+        <v>11</v>
+      </c>
       <c r="H38" s="17"/>
       <c r="K38" s="22"/>
     </row>
-    <row r="39" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="9"/>
-      <c r="H39" s="17"/>
-      <c r="K39" s="22"/>
-    </row>
-    <row r="40" spans="1:14" ht="30.75" thickBot="1">
+    <row r="39" spans="1:14" ht="31.5" thickBot="1">
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" t="s">
+        <v>272</v>
+      </c>
+      <c r="F39" t="s">
+        <v>342</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="I39" t="s">
+        <v>346</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="K39" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+    </row>
+    <row r="40" spans="1:14" ht="44" thickBot="1">
       <c r="C40" t="s">
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>343</v>
+        <v>270</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>345</v>
+        <v>283</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>348</v>
+        <v>281</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>349</v>
+        <v>284</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
     </row>
-    <row r="41" spans="1:14" ht="45.75" thickBot="1">
-      <c r="C41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>275</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="K41" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-    </row>
-    <row r="42" spans="1:14">
+    <row r="41" spans="1:14" ht="16" thickBot="1">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="H41" s="17"/>
+      <c r="K41" s="22"/>
+    </row>
+    <row r="42" spans="1:14" ht="16" thickBot="1">
       <c r="A42" t="s">
-        <v>21</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F42" s="9"/>
       <c r="H42" s="17"/>
       <c r="K42" s="22"/>
+    </row>
+    <row r="43" spans="1:14" ht="29.5" thickBot="1">
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>273</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" ht="44" thickBot="1">
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="17"/>
+      <c r="K45" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2996,23 +3068,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="13.08203125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" s="29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="23.08203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="20.625" customWidth="1"/>
-    <col min="4" max="4" width="30.625" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="3" max="3" width="20.58203125" customWidth="1"/>
+    <col min="4" max="4" width="30.58203125" customWidth="1"/>
+    <col min="5" max="5" width="29.08203125" customWidth="1"/>
     <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -3216,7 +3329,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3250,7 +3363,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3662,7 +3775,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="31.5">
+    <row r="45" spans="1:5" ht="31">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -4144,27 +4257,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.875" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="10" width="43.125" customWidth="1"/>
-    <col min="11" max="11" width="35.125" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.58203125" customWidth="1"/>
+    <col min="7" max="7" width="25.58203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="10" max="10" width="43.08203125" customWidth="1"/>
+    <col min="11" max="11" width="35.08203125" customWidth="1"/>
     <col min="12" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4206,7 +4319,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26.1" customHeight="1">
+    <row r="2" spans="1:12" ht="26.15" customHeight="1">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -4267,7 +4380,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="64.7" customHeight="1">
+    <row r="4" spans="1:12" ht="64.75" customHeight="1">
       <c r="I4" s="1"/>
     </row>
   </sheetData>
@@ -4281,7 +4394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -4289,15 +4402,15 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="5" width="18.375" style="22" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
     <col min="8" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4362,7 +4475,7 @@
       <c r="E5" s="27"/>
       <c r="H5" s="29"/>
     </row>
-    <row r="6" spans="1:8" ht="31.5">
+    <row r="6" spans="1:8" ht="31">
       <c r="A6" s="6" t="s">
         <v>228</v>
       </c>
@@ -4443,7 +4556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -4451,10 +4564,10 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="31.125" customWidth="1"/>
+    <col min="3" max="3" width="31.08203125" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added all as an option for electricity_source and changed text average hours per day
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="500">
   <si>
     <t>clause</t>
   </si>
@@ -1038,15 +1038,6 @@
     <t>display.hint.text.es</t>
   </si>
   <si>
-    <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both_grid_and_generator') || selected(data('electricity_source'), 'both_grid_and_solar'))</t>
-  </si>
-  <si>
-    <t>(hours per day)</t>
-  </si>
-  <si>
-    <t>(horas por día)</t>
-  </si>
-  <si>
     <t>(kilometers)</t>
   </si>
   <si>
@@ -1516,6 +1507,24 @@
   </si>
   <si>
     <t>selected(data('change_admin_region'), 'yes')</t>
+  </si>
+  <si>
+    <t>(average hours per day)</t>
+  </si>
+  <si>
+    <t>(horas promedio por día)</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both_grid_and_generator') || selected(data('electricity_source'), 'both_grid_and_solar') || selected(data('electricity_source'), 'all'))</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1648,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1710,6 +1719,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2146,27 +2158,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="77.5">
       <c r="A3" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -2179,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -2220,7 +2232,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -2229,7 +2241,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>335</v>
@@ -2238,7 +2250,7 @@
         <v>336</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
@@ -2281,7 +2293,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -2290,7 +2302,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2315,7 +2327,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
@@ -2324,7 +2336,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="P4" t="b">
         <f>TRUE()</f>
@@ -2359,7 +2371,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
@@ -2368,7 +2380,7 @@
         <v>24</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="33" customFormat="1">
@@ -2379,27 +2391,27 @@
         <v>56</v>
       </c>
       <c r="E8" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="G8" s="33" t="s">
         <v>490</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="I8" s="33" t="s">
         <v>492</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>493</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>495</v>
-      </c>
       <c r="J8" s="33" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="29" customFormat="1">
       <c r="A9" s="29" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H9" s="30"/>
       <c r="K9" s="30"/>
@@ -2421,7 +2433,7 @@
         <v>28</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I10" t="s">
         <v>27</v>
@@ -2430,7 +2442,7 @@
         <v>28</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -2474,7 +2486,7 @@
         <v>33</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I14" t="s">
         <v>34</v>
@@ -2483,7 +2495,7 @@
         <v>33</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2503,7 +2515,7 @@
         <v>38</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I15" t="s">
         <v>39</v>
@@ -2512,7 +2524,7 @@
         <v>38</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2529,7 +2541,7 @@
         <v>289</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I16" t="s">
         <v>290</v>
@@ -2538,7 +2550,7 @@
         <v>289</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2572,7 +2584,7 @@
         <v>45</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I19" t="s">
         <v>46</v>
@@ -2581,7 +2593,7 @@
         <v>45</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -2589,44 +2601,44 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>337</v>
+        <v>499</v>
       </c>
       <c r="H20" s="17"/>
       <c r="K20" s="22"/>
     </row>
-    <row r="21" spans="1:13">
-      <c r="C21" t="s">
+    <row r="21" spans="1:13" s="33" customFormat="1">
+      <c r="C21" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H21" s="33" t="s">
+        <v>405</v>
+      </c>
+      <c r="I21" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="25" t="s">
-        <v>427</v>
-      </c>
-      <c r="L21" t="s">
-        <v>338</v>
-      </c>
-      <c r="M21" t="s">
-        <v>339</v>
+      <c r="K21" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="M21" s="33" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2653,7 +2665,7 @@
         <v>55</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I23" t="s">
         <v>295</v>
@@ -2662,7 +2674,7 @@
         <v>55</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2679,36 +2691,36 @@
       <c r="H25" s="17"/>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:13" ht="46.5">
-      <c r="C26" t="s">
+    <row r="26" spans="1:13" s="33" customFormat="1" ht="46.5">
+      <c r="C26" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" s="34" t="s">
+        <v>407</v>
+      </c>
+      <c r="I26" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="K26" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="L26" t="s">
-        <v>340</v>
-      </c>
-      <c r="M26" t="s">
-        <v>341</v>
+      <c r="K26" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="L26" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="M26" s="33" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -2728,7 +2740,7 @@
         <v>63</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I27" t="s">
         <v>64</v>
@@ -2737,7 +2749,7 @@
         <v>297</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -2768,7 +2780,7 @@
         <v>67</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I30" t="s">
         <v>296</v>
@@ -2777,7 +2789,7 @@
         <v>298</v>
       </c>
       <c r="K30" s="25" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2797,7 +2809,7 @@
         <v>71</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I31" t="s">
         <v>72</v>
@@ -2806,7 +2818,7 @@
         <v>299</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2837,7 +2849,7 @@
         <v>75</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I34" t="s">
         <v>76</v>
@@ -2846,7 +2858,7 @@
         <v>300</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="31">
@@ -2863,7 +2875,7 @@
         <v>276</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I35" t="s">
         <v>277</v>
@@ -2872,7 +2884,7 @@
         <v>278</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
@@ -2892,7 +2904,7 @@
         <v>279</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I36" t="s">
         <v>269</v>
@@ -2901,7 +2913,7 @@
         <v>280</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
@@ -2929,22 +2941,22 @@
         <v>272</v>
       </c>
       <c r="F39" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G39" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="I39" t="s">
+        <v>343</v>
+      </c>
+      <c r="J39" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="H39" s="20" t="s">
-        <v>417</v>
-      </c>
-      <c r="I39" t="s">
-        <v>346</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>347</v>
-      </c>
       <c r="K39" s="25" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="L39" s="11"/>
       <c r="M39" s="11"/>
@@ -2964,7 +2976,7 @@
         <v>283</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>281</v>
@@ -2973,7 +2985,7 @@
         <v>284</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
@@ -3003,22 +3015,22 @@
         <v>273</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G43" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="I43" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="H43" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>348</v>
-      </c>
       <c r="J43" s="12" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K43" s="26" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
@@ -3038,7 +3050,7 @@
         <v>285</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>282</v>
@@ -3047,7 +3059,7 @@
         <v>286</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
@@ -3088,7 +3100,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3096,7 +3108,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C2" s="29" t="b">
         <v>1</v>
@@ -3109,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -3139,7 +3151,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3156,7 +3168,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3173,7 +3185,7 @@
         <v>83</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3190,7 +3202,7 @@
         <v>86</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3207,7 +3219,7 @@
         <v>89</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3224,7 +3236,7 @@
         <v>92</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3241,7 +3253,7 @@
         <v>95</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3258,7 +3270,7 @@
         <v>98</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3275,7 +3287,7 @@
         <v>101</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3292,7 +3304,7 @@
         <v>104</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3309,7 +3321,7 @@
         <v>107</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3326,7 +3338,7 @@
         <v>110</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.149999999999999" customHeight="1">
@@ -3343,7 +3355,7 @@
         <v>113</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3360,7 +3372,7 @@
         <v>304</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.149999999999999" customHeight="1">
@@ -3377,7 +3389,7 @@
         <v>116</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3394,7 +3406,7 @@
         <v>119</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3416,13 +3428,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="29" customFormat="1">
@@ -3430,13 +3442,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="29" customFormat="1">
@@ -3444,13 +3456,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="29" customFormat="1">
@@ -3458,13 +3470,13 @@
         <v>30</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="29" customFormat="1">
@@ -3472,13 +3484,13 @@
         <v>30</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="29" customFormat="1">
@@ -3486,13 +3498,13 @@
         <v>30</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="29" customFormat="1">
@@ -3500,13 +3512,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="29" customFormat="1">
@@ -3514,13 +3526,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="29" customFormat="1">
@@ -3528,13 +3540,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="29" customFormat="1">
@@ -3542,13 +3554,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="29" customFormat="1">
@@ -3556,13 +3568,13 @@
         <v>30</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C29" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="D29" s="29" t="s">
         <v>472</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="29" customFormat="1">
@@ -3570,13 +3582,13 @@
         <v>30</v>
       </c>
       <c r="B30" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="D30" s="29" t="s">
         <v>467</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>473</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="29" customFormat="1">
@@ -3584,13 +3596,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>468</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>474</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="29" customFormat="1">
@@ -3598,10 +3610,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="29" customFormat="1"/>
@@ -3636,7 +3648,7 @@
         <v>125</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3670,7 +3682,7 @@
         <v>131</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3687,7 +3699,7 @@
         <v>134</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3704,7 +3716,7 @@
         <v>136</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3721,7 +3733,7 @@
         <v>306</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3738,7 +3750,7 @@
         <v>139</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3755,7 +3767,7 @@
         <v>142</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3772,7 +3784,7 @@
         <v>311</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="31">
@@ -3789,41 +3801,39 @@
         <v>319</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="33" customFormat="1">
+      <c r="A46" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="E46" s="34"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
         <v>143</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>144</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" t="s">
-        <v>147</v>
-      </c>
-      <c r="D48" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>378</v>
+      <c r="E47" s="15" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3831,16 +3841,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3848,16 +3858,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3865,16 +3875,16 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C51" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3882,33 +3892,33 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" t="s">
+        <v>157</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
         <v>143</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>144</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>158</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>293</v>
-      </c>
-      <c r="B54" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" t="s">
-        <v>160</v>
-      </c>
-      <c r="D54" t="s">
-        <v>161</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>161</v>
+      <c r="E53" s="15" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3916,16 +3926,16 @@
         <v>293</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>383</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3933,16 +3943,16 @@
         <v>293</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C56" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3950,16 +3960,16 @@
         <v>293</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D57" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3967,33 +3977,33 @@
         <v>293</v>
       </c>
       <c r="B58" t="s">
+        <v>167</v>
+      </c>
+      <c r="C58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>293</v>
+      </c>
+      <c r="B59" t="s">
         <v>170</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>171</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>172</v>
       </c>
-      <c r="E58" s="15" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" t="s">
-        <v>173</v>
-      </c>
-      <c r="C60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" t="s">
-        <v>174</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>387</v>
+      <c r="E59" s="15" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4001,16 +4011,16 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4018,33 +4028,33 @@
         <v>57</v>
       </c>
       <c r="B62" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" t="s">
+        <v>177</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" t="s">
         <v>178</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>179</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>180</v>
       </c>
-      <c r="E62" s="15" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>181</v>
-      </c>
-      <c r="C64" t="s">
-        <v>182</v>
-      </c>
-      <c r="D64" t="s">
-        <v>183</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>390</v>
+      <c r="E63" s="15" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -4052,16 +4062,16 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D65" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -4069,33 +4079,33 @@
         <v>62</v>
       </c>
       <c r="B66" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
         <v>140</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>187</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>188</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
-        <v>292</v>
-      </c>
-      <c r="B68" t="s">
-        <v>189</v>
-      </c>
-      <c r="C68" t="s">
-        <v>313</v>
-      </c>
-      <c r="D68" t="s">
-        <v>317</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>393</v>
+      <c r="E67" s="15" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -4103,16 +4113,16 @@
         <v>292</v>
       </c>
       <c r="B69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C69" t="s">
-        <v>191</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>192</v>
+        <v>313</v>
+      </c>
+      <c r="D69" t="s">
+        <v>317</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -4120,16 +4130,16 @@
         <v>292</v>
       </c>
       <c r="B70" t="s">
-        <v>312</v>
+        <v>190</v>
       </c>
       <c r="C70" t="s">
-        <v>193</v>
-      </c>
-      <c r="D70" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -4137,16 +4147,16 @@
         <v>292</v>
       </c>
       <c r="B71" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>193</v>
       </c>
       <c r="D71" t="s">
-        <v>316</v>
+        <v>194</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4154,33 +4164,33 @@
         <v>292</v>
       </c>
       <c r="B72" t="s">
+        <v>314</v>
+      </c>
+      <c r="C72" t="s">
+        <v>315</v>
+      </c>
+      <c r="D72" t="s">
+        <v>316</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>292</v>
+      </c>
+      <c r="B73" t="s">
         <v>143</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>144</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>145</v>
       </c>
-      <c r="E72" s="15" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74" t="s">
-        <v>196</v>
-      </c>
-      <c r="D74" t="s">
-        <v>197</v>
-      </c>
-      <c r="E74" s="15" t="s">
-        <v>397</v>
+      <c r="E73" s="15" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4188,16 +4198,16 @@
         <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C75" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D75" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4205,16 +4215,16 @@
         <v>68</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D76" t="s">
-        <v>202</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>399</v>
+        <v>200</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4222,16 +4232,16 @@
         <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c r="D77" t="s">
-        <v>158</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>382</v>
+        <v>202</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4239,16 +4249,33 @@
         <v>68</v>
       </c>
       <c r="B78" t="s">
+        <v>143</v>
+      </c>
+      <c r="C78" t="s">
+        <v>144</v>
+      </c>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" t="s">
         <v>167</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>168</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>169</v>
       </c>
-      <c r="E78" s="15" t="s">
-        <v>385</v>
+      <c r="E79" s="15" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4316,7 +4343,7 @@
         <v>213</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="26.15" customHeight="1">
@@ -4377,7 +4404,7 @@
         <v>220</v>
       </c>
       <c r="L3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="64.75" customHeight="1">
@@ -4428,7 +4455,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F1" t="s">
         <v>223</v>
@@ -4437,7 +4464,7 @@
         <v>224</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4461,7 +4488,7 @@
         <v>323</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H4" s="29"/>
     </row>
@@ -4518,7 +4545,7 @@
         <v>233</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4533,21 +4560,21 @@
         <v>236</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>434</v>
+      </c>
+      <c r="F11" t="s">
+        <v>435</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="H11" s="29" t="s">
         <v>437</v>
-      </c>
-      <c r="F11" t="s">
-        <v>438</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>439</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added number of spare fuel cylinders available question
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="506">
   <si>
     <t>clause</t>
   </si>
@@ -1525,6 +1525,25 @@
   </si>
   <si>
     <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both_grid_and_generator') || selected(data('electricity_source'), 'both_grid_and_solar') || selected(data('electricity_source'), 'all'))</t>
+  </si>
+  <si>
+    <t>spare_fuel_cylinders_available</t>
+  </si>
+  <si>
+    <t>Number of spare fuel cylinders available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Número de cilindros de combustible de repuesto disponibles</t>
+  </si>
+  <si>
+    <t>Contact Phone Number?</t>
+  </si>
+  <si>
+    <t>Number of spare fuel cylinders available?</t>
+  </si>
+  <si>
+    <t>Número de cilindros de combustible de repuesto disponibles?</t>
   </si>
 </sst>
 </file>
@@ -2189,10 +2208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -2907,7 +2926,7 @@
         <v>413</v>
       </c>
       <c r="I36" t="s">
-        <v>269</v>
+        <v>503</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>280</v>
@@ -2926,151 +2945,171 @@
       <c r="H37" s="17"/>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="1:14">
-      <c r="A38" t="s">
+    <row r="38" spans="1:14" s="33" customFormat="1" ht="46.5">
+      <c r="C38" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>500</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>501</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>502</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="17"/>
-      <c r="K38" s="22"/>
-    </row>
-    <row r="39" spans="1:14" ht="31.5" thickBot="1">
-      <c r="C39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" t="s">
-        <v>272</v>
-      </c>
-      <c r="F39" t="s">
-        <v>339</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>414</v>
-      </c>
-      <c r="I39" t="s">
-        <v>343</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K39" s="25" t="s">
-        <v>414</v>
-      </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-    </row>
-    <row r="40" spans="1:14" ht="44" thickBot="1">
+      <c r="H39" s="17"/>
+      <c r="K39" s="22"/>
+    </row>
+    <row r="40" spans="1:14" ht="31.5" thickBot="1">
       <c r="C40" t="s">
         <v>40</v>
       </c>
       <c r="E40" t="s">
+        <v>272</v>
+      </c>
+      <c r="F40" t="s">
+        <v>339</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="I40" t="s">
+        <v>343</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+    </row>
+    <row r="41" spans="1:14" ht="44" thickBot="1">
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
         <v>274</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G41" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H41" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="J40" s="12" t="s">
+      <c r="J41" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="K40" s="26" t="s">
+      <c r="K41" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-    </row>
-    <row r="41" spans="1:14" ht="16" thickBot="1">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" s="9"/>
-      <c r="H41" s="17"/>
-      <c r="K41" s="22"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
     </row>
     <row r="42" spans="1:14" ht="16" thickBot="1">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F42" s="9"/>
       <c r="H42" s="17"/>
       <c r="K42" s="22"/>
     </row>
-    <row r="43" spans="1:14" ht="29.5" thickBot="1">
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" t="s">
-        <v>273</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="H43" s="21" t="s">
-        <v>415</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="K43" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-    </row>
-    <row r="44" spans="1:14" ht="44" thickBot="1">
+    <row r="43" spans="1:14" ht="16" thickBot="1">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="H43" s="17"/>
+      <c r="K43" s="22"/>
+    </row>
+    <row r="44" spans="1:14" ht="29.5" thickBot="1">
       <c r="C44" t="s">
         <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>271</v>
+        <v>340</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>282</v>
+        <v>345</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>286</v>
+        <v>346</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14">
-      <c r="A45" t="s">
+    <row r="45" spans="1:14" ht="44" thickBot="1">
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>275</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J45" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="K45" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
         <v>21</v>
       </c>
-      <c r="H45" s="17"/>
-      <c r="K45" s="22"/>
+      <c r="H46" s="17"/>
+      <c r="K46" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add 0.3l, 0.4l, 0.6l ice packs
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="521">
   <si>
     <t>clause</t>
   </si>
@@ -1544,6 +1544,51 @@
   </si>
   <si>
     <t>Número de cilindros de combustible de repuesto disponibles?</t>
+  </si>
+  <si>
+    <t>number_of_l3_packs</t>
+  </si>
+  <si>
+    <t>number_of_l4_packs</t>
+  </si>
+  <si>
+    <t>Number of 0.3 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Number of 0.4 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.3 litros</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.4 litros</t>
+  </si>
+  <si>
+    <t>number_of_l6_packs</t>
+  </si>
+  <si>
+    <t>Number of 0.6 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.6 litros</t>
+  </si>
+  <si>
+    <t>Total number of 0.3 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.3 litros?</t>
+  </si>
+  <si>
+    <t>Total number of 0.4 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Total number of 0.6 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.4 litros?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.6 litros?</t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -3110,6 +3155,76 @@
       </c>
       <c r="H46" s="17"/>
       <c r="K46" s="22"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="33" customFormat="1">
+      <c r="C48" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>506</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>508</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>510</v>
+      </c>
+      <c r="I48" s="33" t="s">
+        <v>515</v>
+      </c>
+      <c r="J48" s="33" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="33" customFormat="1">
+      <c r="C49" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>507</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>509</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>511</v>
+      </c>
+      <c r="I49" s="33" t="s">
+        <v>517</v>
+      </c>
+      <c r="J49" s="33" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="33" customFormat="1">
+      <c r="C50" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>512</v>
+      </c>
+      <c r="F50" s="33" t="s">
+        <v>513</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>514</v>
+      </c>
+      <c r="I50" s="33" t="s">
+        <v>518</v>
+      </c>
+      <c r="J50" s="33" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add question for spare temp monitoring devices
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="526">
   <si>
     <t>clause</t>
   </si>
@@ -1527,16 +1527,9 @@
     <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both_grid_and_generator') || selected(data('electricity_source'), 'both_grid_and_solar') || selected(data('electricity_source'), 'all'))</t>
   </si>
   <si>
-    <t>spare_fuel_cylinders_available</t>
-  </si>
-  <si>
     <t>Number of spare fuel cylinders available</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Número de cilindros de combustible de repuesto disponibles</t>
-  </si>
-  <si>
     <t>Contact Phone Number?</t>
   </si>
   <si>
@@ -1589,6 +1582,27 @@
   </si>
   <si>
     <t>Número total de paquetes de hielo/agua de 0.6 litros?</t>
+  </si>
+  <si>
+    <t>spare_temp_monitoring_devices</t>
+  </si>
+  <si>
+    <t>spare_fuel_cylinders</t>
+  </si>
+  <si>
+    <t>Number of spare/replacement temperature monitoring devices</t>
+  </si>
+  <si>
+    <t>Número de dispositivos de monitoreo de temperatura de repuesto/reemplazo</t>
+  </si>
+  <si>
+    <t>Number of spare/replacement temperature monitoring devices?</t>
+  </si>
+  <si>
+    <t>Número de dispositivos de monitoreo de temperatura de repuesto/reemplazo?</t>
+  </si>
+  <si>
+    <t>Número de cilindros de combustible de repuesto disponibles</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1726,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1786,6 +1800,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2253,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
@@ -2971,7 +2986,7 @@
         <v>413</v>
       </c>
       <c r="I36" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="J36" s="11" t="s">
         <v>280</v>
@@ -2990,239 +3005,271 @@
       <c r="H37" s="17"/>
       <c r="K37" s="22"/>
     </row>
-    <row r="38" spans="1:14" s="33" customFormat="1" ht="46.5">
-      <c r="C38" s="33" t="s">
+    <row r="38" spans="1:14" s="29" customFormat="1">
+      <c r="A38" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="35" customFormat="1" ht="20" customHeight="1">
+      <c r="C39" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E39" s="35" t="s">
+        <v>520</v>
+      </c>
+      <c r="F39" s="35" t="s">
         <v>500</v>
       </c>
-      <c r="F38" s="33" t="s">
-        <v>501</v>
-      </c>
-      <c r="G38" s="34" t="s">
+      <c r="G39" s="35" t="s">
+        <v>525</v>
+      </c>
+      <c r="I39" s="35" t="s">
         <v>502</v>
       </c>
-      <c r="I38" s="33" t="s">
-        <v>504</v>
-      </c>
-      <c r="J38" s="34" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" t="s">
+      <c r="J39" s="35" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="35" customFormat="1" ht="19" customHeight="1">
+      <c r="C40" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>521</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>522</v>
+      </c>
+      <c r="I40" s="35" t="s">
+        <v>523</v>
+      </c>
+      <c r="J40" s="35" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="30" customFormat="1">
+      <c r="A41" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="J41" s="25"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="17"/>
-      <c r="K39" s="22"/>
-    </row>
-    <row r="40" spans="1:14" ht="31.5" thickBot="1">
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" t="s">
-        <v>272</v>
-      </c>
-      <c r="F40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>414</v>
-      </c>
-      <c r="I40" t="s">
-        <v>343</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K40" s="25" t="s">
-        <v>414</v>
-      </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-    </row>
-    <row r="41" spans="1:14" ht="44" thickBot="1">
-      <c r="C41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" t="s">
-        <v>274</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>416</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="K41" s="26" t="s">
-        <v>416</v>
-      </c>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-    </row>
-    <row r="42" spans="1:14" ht="16" thickBot="1">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="9"/>
       <c r="H42" s="17"/>
       <c r="K42" s="22"/>
     </row>
-    <row r="43" spans="1:14" ht="16" thickBot="1">
-      <c r="A43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="H43" s="17"/>
-      <c r="K43" s="22"/>
-    </row>
-    <row r="44" spans="1:14" ht="29.5" thickBot="1">
+    <row r="43" spans="1:14" ht="31.5" thickBot="1">
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>272</v>
+      </c>
+      <c r="F43" t="s">
+        <v>339</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="H43" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="I43" t="s">
+        <v>343</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="K43" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+    </row>
+    <row r="44" spans="1:14" ht="44" thickBot="1">
       <c r="C44" t="s">
         <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>342</v>
+        <v>283</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>345</v>
+        <v>281</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>346</v>
+        <v>284</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14" ht="44" thickBot="1">
-      <c r="C45" t="s">
-        <v>40</v>
-      </c>
-      <c r="E45" t="s">
-        <v>275</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>417</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="J45" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="K45" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-    </row>
-    <row r="46" spans="1:14">
+    <row r="45" spans="1:14" ht="16" thickBot="1">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="H45" s="17"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="1:14" ht="16" thickBot="1">
       <c r="A46" t="s">
-        <v>21</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F46" s="9"/>
       <c r="H46" s="17"/>
       <c r="K46" s="22"/>
     </row>
-    <row r="47" spans="1:14">
-      <c r="A47" t="s">
+    <row r="47" spans="1:14" ht="29.5" thickBot="1">
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>273</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="K47" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" ht="44" thickBot="1">
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" t="s">
+        <v>275</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="K48" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="33" customFormat="1">
-      <c r="C48" s="33" t="s">
+    <row r="51" spans="1:11" s="33" customFormat="1">
+      <c r="C51" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E51" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="F51" s="33" t="s">
         <v>506</v>
       </c>
-      <c r="F48" s="33" t="s">
+      <c r="G51" s="33" t="s">
         <v>508</v>
       </c>
-      <c r="G48" s="33" t="s">
+      <c r="I51" s="33" t="s">
+        <v>513</v>
+      </c>
+      <c r="J51" s="33" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="33" customFormat="1">
+      <c r="C52" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>505</v>
+      </c>
+      <c r="F52" s="33" t="s">
+        <v>507</v>
+      </c>
+      <c r="G52" s="33" t="s">
+        <v>509</v>
+      </c>
+      <c r="I52" s="33" t="s">
+        <v>515</v>
+      </c>
+      <c r="J52" s="33" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="33" customFormat="1">
+      <c r="C53" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="33" t="s">
         <v>510</v>
       </c>
-      <c r="I48" s="33" t="s">
-        <v>515</v>
-      </c>
-      <c r="J48" s="33" t="s">
+      <c r="F53" s="33" t="s">
+        <v>511</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>512</v>
+      </c>
+      <c r="I53" s="33" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" s="33" customFormat="1">
-      <c r="C49" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="33" t="s">
-        <v>507</v>
-      </c>
-      <c r="F49" s="33" t="s">
-        <v>509</v>
-      </c>
-      <c r="G49" s="33" t="s">
-        <v>511</v>
-      </c>
-      <c r="I49" s="33" t="s">
-        <v>517</v>
-      </c>
-      <c r="J49" s="33" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="33" customFormat="1">
-      <c r="C50" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="33" t="s">
-        <v>512</v>
-      </c>
-      <c r="F50" s="33" t="s">
-        <v>513</v>
-      </c>
-      <c r="G50" s="33" t="s">
-        <v>514</v>
-      </c>
-      <c r="I50" s="33" t="s">
+      <c r="J53" s="33" t="s">
         <v>518</v>
       </c>
-      <c r="J50" s="33" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" t="s">
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create and use customCCEGroups
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2508" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="529">
   <si>
     <t>clause</t>
   </si>
@@ -1603,6 +1603,15 @@
   </si>
   <si>
     <t>Número de cilindros de combustible de repuesto disponibles</t>
+  </si>
+  <si>
+    <t>cceGroupPrivileged</t>
+  </si>
+  <si>
+    <t>cceGroupModify</t>
+  </si>
+  <si>
+    <t>cceGroupReadOnly</t>
   </si>
 </sst>
 </file>
@@ -2220,13 +2229,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="16" style="29" customWidth="1"/>
-    <col min="2" max="2" width="8.75" style="29"/>
+    <col min="2" max="2" width="8.69921875" style="29"/>
     <col min="3" max="3" width="18" style="29" customWidth="1"/>
-    <col min="4" max="4" width="24.25" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="8.75" style="29"/>
+    <col min="4" max="4" width="24.19921875" style="29" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2250,7 +2259,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5">
+    <row r="3" spans="1:4" ht="78">
       <c r="A3" s="1" t="s">
         <v>441</v>
       </c>
@@ -2270,21 +2279,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.58203125" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" customWidth="1"/>
+    <col min="5" max="5" width="35.59765625" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
-    <col min="7" max="7" width="33.83203125" customWidth="1"/>
-    <col min="8" max="9" width="26.83203125" customWidth="1"/>
-    <col min="10" max="15" width="47.58203125" customWidth="1"/>
+    <col min="7" max="7" width="33.796875" customWidth="1"/>
+    <col min="8" max="9" width="26.796875" customWidth="1"/>
+    <col min="10" max="15" width="47.59765625" customWidth="1"/>
     <col min="16" max="1030" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2357,7 +2366,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="25" customHeight="1">
+    <row r="3" spans="1:16" ht="25.05" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2770,7 +2779,7 @@
       <c r="H25" s="17"/>
       <c r="K25" s="22"/>
     </row>
-    <row r="26" spans="1:13" s="33" customFormat="1" ht="46.5">
+    <row r="26" spans="1:13" s="33" customFormat="1" ht="46.8">
       <c r="C26" s="33" t="s">
         <v>41</v>
       </c>
@@ -2845,7 +2854,7 @@
       <c r="H29" s="17"/>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" spans="1:13" ht="31">
+    <row r="30" spans="1:13" ht="31.2">
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -2914,7 +2923,7 @@
       <c r="H33" s="17"/>
       <c r="K33" s="22"/>
     </row>
-    <row r="34" spans="1:14" ht="31">
+    <row r="34" spans="1:14" ht="31.2">
       <c r="C34" t="s">
         <v>12</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="31">
+    <row r="35" spans="1:14" ht="31.2">
       <c r="C35" t="s">
         <v>12</v>
       </c>
@@ -2969,7 +2978,7 @@
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
     </row>
-    <row r="36" spans="1:14" ht="31">
+    <row r="36" spans="1:14" ht="31.2">
       <c r="C36" t="s">
         <v>12</v>
       </c>
@@ -3010,7 +3019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="35" customFormat="1" ht="20" customHeight="1">
+    <row r="39" spans="1:14" s="35" customFormat="1" ht="19.95" customHeight="1">
       <c r="C39" s="35" t="s">
         <v>40</v>
       </c>
@@ -3030,7 +3039,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="40" spans="1:14" s="35" customFormat="1" ht="19.05" customHeight="1">
       <c r="C40" s="35" t="s">
         <v>40</v>
       </c>
@@ -3064,7 +3073,7 @@
       <c r="H42" s="17"/>
       <c r="K42" s="22"/>
     </row>
-    <row r="43" spans="1:14" ht="31.5" thickBot="1">
+    <row r="43" spans="1:14" ht="31.8" thickBot="1">
       <c r="C43" t="s">
         <v>40</v>
       </c>
@@ -3093,7 +3102,7 @@
       <c r="M43" s="11"/>
       <c r="N43" s="11"/>
     </row>
-    <row r="44" spans="1:14" ht="44" thickBot="1">
+    <row r="44" spans="1:14" ht="43.8" thickBot="1">
       <c r="C44" t="s">
         <v>40</v>
       </c>
@@ -3122,7 +3131,7 @@
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14" ht="16" thickBot="1">
+    <row r="45" spans="1:14" ht="16.2" thickBot="1">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -3130,7 +3139,7 @@
       <c r="H45" s="17"/>
       <c r="K45" s="22"/>
     </row>
-    <row r="46" spans="1:14" ht="16" thickBot="1">
+    <row r="46" spans="1:14" ht="16.2" thickBot="1">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3138,7 +3147,7 @@
       <c r="H46" s="17"/>
       <c r="K46" s="22"/>
     </row>
-    <row r="47" spans="1:14" ht="29.5" thickBot="1">
+    <row r="47" spans="1:14" ht="29.4" thickBot="1">
       <c r="C47" t="s">
         <v>40</v>
       </c>
@@ -3167,7 +3176,7 @@
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
     </row>
-    <row r="48" spans="1:14" ht="44" thickBot="1">
+    <row r="48" spans="1:14" ht="43.8" thickBot="1">
       <c r="C48" t="s">
         <v>40</v>
       </c>
@@ -3281,16 +3290,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" customWidth="1"/>
+    <col min="2" max="2" width="24.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3313,6 +3322,30 @@
       </c>
       <c r="C2" s="29" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -3328,17 +3361,17 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="23.08203125" customWidth="1"/>
+    <col min="1" max="1" width="23.09765625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" customWidth="1"/>
-    <col min="4" max="4" width="30.58203125" customWidth="1"/>
-    <col min="5" max="5" width="29.08203125" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" customWidth="1"/>
+    <col min="4" max="4" width="30.59765625" customWidth="1"/>
+    <col min="5" max="5" width="29.09765625" customWidth="1"/>
     <col min="6" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -3542,7 +3575,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3576,7 +3609,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3988,7 +4021,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="31">
+    <row r="45" spans="1:5" ht="31.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -4493,19 +4526,19 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.296875" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.58203125" customWidth="1"/>
-    <col min="7" max="7" width="25.58203125" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" customWidth="1"/>
-    <col min="10" max="10" width="43.08203125" customWidth="1"/>
-    <col min="11" max="11" width="35.08203125" customWidth="1"/>
+    <col min="5" max="5" width="29.796875" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" customWidth="1"/>
+    <col min="8" max="8" width="15.296875" customWidth="1"/>
+    <col min="9" max="9" width="23.296875" customWidth="1"/>
+    <col min="10" max="10" width="43.09765625" customWidth="1"/>
+    <col min="11" max="11" width="35.09765625" customWidth="1"/>
     <col min="12" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4547,7 +4580,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26.15" customHeight="1">
+    <row r="2" spans="1:12" ht="26.1" customHeight="1">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -4608,7 +4641,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="64.75" customHeight="1">
+    <row r="4" spans="1:12" ht="64.8" customHeight="1">
       <c r="I4" s="1"/>
     </row>
   </sheetData>
@@ -4630,15 +4663,15 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" customWidth="1"/>
+    <col min="5" max="5" width="18.296875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="18.796875" customWidth="1"/>
     <col min="8" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4703,7 +4736,7 @@
       <c r="E5" s="27"/>
       <c r="H5" s="29"/>
     </row>
-    <row r="6" spans="1:8" ht="31">
+    <row r="6" spans="1:8" ht="31.2">
       <c r="A6" s="6" t="s">
         <v>228</v>
       </c>
@@ -4792,10 +4825,10 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="31.08203125" customWidth="1"/>
+    <col min="3" max="3" width="31.09765625" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Change spare fuel cylinders available to stand-by gas cylinders
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="531">
   <si>
     <t>clause</t>
   </si>
@@ -1512,18 +1512,9 @@
     <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both_grid_and_generator') || selected(data('electricity_source'), 'both_grid_and_solar') || selected(data('electricity_source'), 'all'))</t>
   </si>
   <si>
-    <t>Number of spare fuel cylinders available</t>
-  </si>
-  <si>
     <t>Contact Phone Number?</t>
   </si>
   <si>
-    <t>Number of spare fuel cylinders available?</t>
-  </si>
-  <si>
-    <t>Número de cilindros de combustible de repuesto disponibles?</t>
-  </si>
-  <si>
     <t>number_of_l3_packs</t>
   </si>
   <si>
@@ -1587,9 +1578,6 @@
     <t>Número de dispositivos de monitoreo de temperatura de repuesto/reemplazo?</t>
   </si>
   <si>
-    <t>Número de cilindros de combustible de repuesto disponibles</t>
-  </si>
-  <si>
     <t>cceGroupPrivileged</t>
   </si>
   <si>
@@ -1624,6 +1612,12 @@
   </si>
   <si>
     <t>Choose the gas cylinder availability</t>
+  </si>
+  <si>
+    <t>Número de cilindros de gas de reserva disponibles, si corresponde</t>
+  </si>
+  <si>
+    <t>Number of stand-by gas cylinders available, if applicable</t>
   </si>
 </sst>
 </file>
@@ -2291,8 +2285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K8" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -2359,16 +2353,16 @@
         <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="29" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2382,7 +2376,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="29" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2785,22 +2779,22 @@
         <v>54</v>
       </c>
       <c r="F24" t="s">
+        <v>524</v>
+      </c>
+      <c r="G24" t="s">
+        <v>525</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="I24" t="s">
         <v>528</v>
       </c>
-      <c r="G24" t="s">
-        <v>529</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>530</v>
-      </c>
-      <c r="I24" t="s">
-        <v>532</v>
-      </c>
       <c r="J24" t="s">
+        <v>523</v>
+      </c>
+      <c r="K24" s="25" t="s">
         <v>527</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3033,7 +3027,7 @@
         <v>409</v>
       </c>
       <c r="I37" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J37" s="11" t="s">
         <v>279</v>
@@ -3062,19 +3056,19 @@
         <v>40</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>495</v>
+        <v>530</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>497</v>
+        <v>530</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>498</v>
+        <v>529</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="35" customFormat="1" ht="19.05" customHeight="1">
@@ -3082,19 +3076,19 @@
         <v>40</v>
       </c>
       <c r="E41" s="35" t="s">
+        <v>511</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>513</v>
+      </c>
+      <c r="G41" s="35" t="s">
         <v>514</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="I41" s="35" t="s">
+        <v>515</v>
+      </c>
+      <c r="J41" s="35" t="s">
         <v>516</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>517</v>
-      </c>
-      <c r="I41" s="35" t="s">
-        <v>518</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="30" customFormat="1">
@@ -3260,19 +3254,19 @@
         <v>40</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I52" s="33" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="J52" s="33" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="33" customFormat="1">
@@ -3280,19 +3274,19 @@
         <v>40</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="54" spans="1:14" s="33" customFormat="1">
@@ -3300,19 +3294,19 @@
         <v>40</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F54" s="33" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I54" s="33" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="J54" s="33" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3367,7 +3361,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3375,7 +3369,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3383,7 +3377,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add usable to total number of cold boxes at facility
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="532">
   <si>
     <t>clause</t>
   </si>
@@ -1035,24 +1035,12 @@
     <t>(kilómetros)</t>
   </si>
   <si>
-    <t>Total number of cold boxes at facility</t>
-  </si>
-  <si>
     <t>Total number of vaccine carriers at facility</t>
   </si>
   <si>
-    <t>Número total de cajas frías en la facilidad</t>
-  </si>
-  <si>
     <t>Número total de portadores de vacunas en la facilidad</t>
   </si>
   <si>
-    <t>Total number of cold boxes at facility?</t>
-  </si>
-  <si>
-    <t>Número total de cajas frías en la facilidad?</t>
-  </si>
-  <si>
     <t>Total number of vaccine carriers at facility?</t>
   </si>
   <si>
@@ -1257,9 +1245,6 @@
     <t>Numéro de téléphone de la personne à contacter</t>
   </si>
   <si>
-    <t>Nombre de glacières dans l'établissement</t>
-  </si>
-  <si>
     <t>Nombre de porte-vaccins dans l'établissement</t>
   </si>
   <si>
@@ -1618,6 +1603,24 @@
   </si>
   <si>
     <t>Number of stand-by gas cylinders available, if applicable</t>
+  </si>
+  <si>
+    <t>Total number of usable cold boxes at facility</t>
+  </si>
+  <si>
+    <t>Número total de cajas frías utilizables en la facilidad</t>
+  </si>
+  <si>
+    <t>Nombre total de glacières utilisables dans l'installation</t>
+  </si>
+  <si>
+    <t>Total number of usable cold boxes at facility?</t>
+  </si>
+  <si>
+    <t>Número total de cajas frías utilizables en la facilidad?</t>
+  </si>
+  <si>
+    <t>Nombre total de glacières utilisables dans l'installation?</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1744,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1816,6 +1819,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2252,27 +2256,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="78">
       <c r="A3" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -2285,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="K35" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -2326,7 +2330,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -2335,7 +2339,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>332</v>
@@ -2344,7 +2348,7 @@
         <v>333</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
@@ -2353,16 +2357,16 @@
         <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="29" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2376,7 +2380,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="29" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2413,7 +2417,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -2422,7 +2426,7 @@
         <v>15</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2447,7 +2451,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
@@ -2456,7 +2460,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="P5" t="b">
         <f>TRUE()</f>
@@ -2491,7 +2495,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
@@ -2500,7 +2504,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="33" customFormat="1">
@@ -2511,27 +2515,27 @@
         <v>55</v>
       </c>
       <c r="E9" s="33" t="s">
+        <v>477</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="I9" s="33" t="s">
         <v>482</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>484</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>485</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>487</v>
-      </c>
       <c r="J9" s="33" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="29" customFormat="1">
       <c r="A10" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>483</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>488</v>
       </c>
       <c r="H10" s="30"/>
       <c r="K10" s="30"/>
@@ -2553,7 +2557,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I11" t="s">
         <v>27</v>
@@ -2562,7 +2566,7 @@
         <v>28</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="P11">
         <v>1</v>
@@ -2606,7 +2610,7 @@
         <v>33</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I15" t="s">
         <v>34</v>
@@ -2615,7 +2619,7 @@
         <v>33</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2635,7 +2639,7 @@
         <v>38</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="I16" t="s">
         <v>39</v>
@@ -2644,7 +2648,7 @@
         <v>38</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2661,7 +2665,7 @@
         <v>288</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I17" t="s">
         <v>289</v>
@@ -2670,7 +2674,7 @@
         <v>288</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -2704,7 +2708,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
@@ -2713,7 +2717,7 @@
         <v>45</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -2721,7 +2725,7 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="H21" s="17"/>
       <c r="K21" s="22"/>
@@ -2743,7 +2747,7 @@
         <v>51</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I22" s="33" t="s">
         <v>52</v>
@@ -2752,13 +2756,13 @@
         <v>51</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="L22" s="33" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="M22" s="33" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2768,33 +2772,33 @@
       <c r="H23" s="17"/>
       <c r="K23" s="22"/>
     </row>
-    <row r="24" spans="1:13">
-      <c r="C24" t="s">
+    <row r="24" spans="1:13" s="33" customFormat="1">
+      <c r="C24" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
-        <v>524</v>
-      </c>
-      <c r="G24" t="s">
-        <v>525</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>526</v>
-      </c>
-      <c r="I24" t="s">
-        <v>528</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="F24" s="33" t="s">
+        <v>519</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>520</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>521</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>523</v>
       </c>
-      <c r="K24" s="25" t="s">
-        <v>527</v>
+      <c r="J24" s="33" t="s">
+        <v>518</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2825,7 +2829,7 @@
         <v>59</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I27" s="33" t="s">
         <v>60</v>
@@ -2834,7 +2838,7 @@
         <v>298</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="L27" s="33" t="s">
         <v>334</v>
@@ -2860,7 +2864,7 @@
         <v>62</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I28" t="s">
         <v>63</v>
@@ -2869,7 +2873,7 @@
         <v>294</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2900,7 +2904,7 @@
         <v>66</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I31" t="s">
         <v>293</v>
@@ -2909,7 +2913,7 @@
         <v>295</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2929,7 +2933,7 @@
         <v>70</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I32" t="s">
         <v>71</v>
@@ -2938,7 +2942,7 @@
         <v>296</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2969,7 +2973,7 @@
         <v>74</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="I35" t="s">
         <v>75</v>
@@ -2978,7 +2982,7 @@
         <v>297</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="31.2">
@@ -2995,7 +2999,7 @@
         <v>275</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="I36" t="s">
         <v>276</v>
@@ -3004,7 +3008,7 @@
         <v>277</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
@@ -3024,16 +3028,16 @@
         <v>278</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="I37" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="J37" s="11" t="s">
         <v>279</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
@@ -3056,19 +3060,19 @@
         <v>40</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="35" customFormat="1" ht="19.05" customHeight="1">
@@ -3076,19 +3080,19 @@
         <v>40</v>
       </c>
       <c r="E41" s="35" t="s">
+        <v>506</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>508</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>509</v>
+      </c>
+      <c r="I41" s="35" t="s">
+        <v>510</v>
+      </c>
+      <c r="J41" s="35" t="s">
         <v>511</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>513</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>514</v>
-      </c>
-      <c r="I41" s="35" t="s">
-        <v>515</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="30" customFormat="1">
@@ -3105,34 +3109,34 @@
       <c r="H43" s="17"/>
       <c r="K43" s="22"/>
     </row>
-    <row r="44" spans="1:14" ht="31.8" thickBot="1">
-      <c r="C44" t="s">
+    <row r="44" spans="1:14" s="33" customFormat="1" ht="31.8" thickBot="1">
+      <c r="C44" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="F44" t="s">
-        <v>336</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="H44" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="I44" t="s">
-        <v>340</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="K44" s="25" t="s">
-        <v>410</v>
-      </c>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
+      <c r="F44" s="33" t="s">
+        <v>526</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>527</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>528</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>529</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="K44" s="34" t="s">
+        <v>531</v>
+      </c>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
     </row>
     <row r="45" spans="1:14" ht="43.8" thickBot="1">
       <c r="C45" t="s">
@@ -3148,7 +3152,7 @@
         <v>282</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>280</v>
@@ -3157,7 +3161,7 @@
         <v>283</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
@@ -3187,22 +3191,22 @@
         <v>272</v>
       </c>
       <c r="F48" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G48" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="H48" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="J48" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="H48" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>343</v>
-      </c>
       <c r="K48" s="26" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
@@ -3222,7 +3226,7 @@
         <v>284</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="I49" s="9" t="s">
         <v>281</v>
@@ -3231,7 +3235,7 @@
         <v>285</v>
       </c>
       <c r="K49" s="26" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
@@ -3254,19 +3258,19 @@
         <v>40</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="G52" s="33" t="s">
+        <v>495</v>
+      </c>
+      <c r="I52" s="33" t="s">
         <v>500</v>
       </c>
-      <c r="I52" s="33" t="s">
-        <v>505</v>
-      </c>
       <c r="J52" s="33" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="33" customFormat="1">
@@ -3274,19 +3278,19 @@
         <v>40</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="54" spans="1:14" s="33" customFormat="1">
@@ -3294,19 +3298,19 @@
         <v>40</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="F54" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>499</v>
+      </c>
+      <c r="I54" s="33" t="s">
         <v>503</v>
       </c>
-      <c r="G54" s="33" t="s">
-        <v>504</v>
-      </c>
-      <c r="I54" s="33" t="s">
-        <v>508</v>
-      </c>
       <c r="J54" s="33" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3342,7 +3346,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3350,7 +3354,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C2" s="29" t="b">
         <v>1</v>
@@ -3361,7 +3365,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3369,7 +3373,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3377,7 +3381,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -3417,7 +3421,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3434,7 +3438,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3451,7 +3455,7 @@
         <v>82</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3468,7 +3472,7 @@
         <v>85</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3485,7 +3489,7 @@
         <v>88</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3502,7 +3506,7 @@
         <v>91</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3519,7 +3523,7 @@
         <v>94</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3536,7 +3540,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3553,7 +3557,7 @@
         <v>100</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3570,7 +3574,7 @@
         <v>103</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3587,7 +3591,7 @@
         <v>106</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3604,7 +3608,7 @@
         <v>109</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
@@ -3621,7 +3625,7 @@
         <v>112</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3638,7 +3642,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
@@ -3655,7 +3659,7 @@
         <v>115</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3672,7 +3676,7 @@
         <v>118</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3694,13 +3698,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="29" customFormat="1">
@@ -3708,13 +3712,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="29" customFormat="1">
@@ -3722,13 +3726,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="29" customFormat="1">
@@ -3736,13 +3740,13 @@
         <v>30</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="29" customFormat="1">
@@ -3750,13 +3754,13 @@
         <v>30</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="29" customFormat="1">
@@ -3764,13 +3768,13 @@
         <v>30</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="29" customFormat="1">
@@ -3778,13 +3782,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="29" customFormat="1">
@@ -3792,13 +3796,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="29" customFormat="1">
@@ -3806,13 +3810,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="29" customFormat="1">
@@ -3820,13 +3824,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="29" customFormat="1">
@@ -3834,13 +3838,13 @@
         <v>30</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="29" customFormat="1">
@@ -3848,13 +3852,13 @@
         <v>30</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="29" customFormat="1">
@@ -3862,13 +3866,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="29" customFormat="1">
@@ -3876,10 +3880,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="29" customFormat="1"/>
@@ -3914,7 +3918,7 @@
         <v>124</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3948,7 +3952,7 @@
         <v>130</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3965,7 +3969,7 @@
         <v>133</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3982,7 +3986,7 @@
         <v>135</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3999,7 +4003,7 @@
         <v>303</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4016,7 +4020,7 @@
         <v>138</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -4033,7 +4037,7 @@
         <v>141</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -4050,7 +4054,7 @@
         <v>308</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="31.2">
@@ -4067,7 +4071,7 @@
         <v>316</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="33" customFormat="1">
@@ -4075,13 +4079,13 @@
         <v>42</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E46" s="34"/>
     </row>
@@ -4099,7 +4103,7 @@
         <v>144</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4116,7 +4120,7 @@
         <v>147</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -4133,7 +4137,7 @@
         <v>150</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -4150,7 +4154,7 @@
         <v>153</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -4167,7 +4171,7 @@
         <v>156</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -4184,7 +4188,7 @@
         <v>157</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4218,7 +4222,7 @@
         <v>162</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -4235,7 +4239,7 @@
         <v>165</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -4252,7 +4256,7 @@
         <v>168</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -4269,7 +4273,7 @@
         <v>171</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4286,7 +4290,7 @@
         <v>173</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4303,7 +4307,7 @@
         <v>176</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -4320,7 +4324,7 @@
         <v>179</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -4337,7 +4341,7 @@
         <v>182</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -4354,7 +4358,7 @@
         <v>185</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -4371,7 +4375,7 @@
         <v>187</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -4388,7 +4392,7 @@
         <v>314</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -4405,7 +4409,7 @@
         <v>191</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -4422,7 +4426,7 @@
         <v>193</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4439,7 +4443,7 @@
         <v>313</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -4456,7 +4460,7 @@
         <v>144</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4473,7 +4477,7 @@
         <v>196</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4490,7 +4494,7 @@
         <v>199</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4507,7 +4511,7 @@
         <v>201</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4524,7 +4528,7 @@
         <v>157</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4541,7 +4545,7 @@
         <v>168</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -4609,7 +4613,7 @@
         <v>212</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="26.1" customHeight="1">
@@ -4670,7 +4674,7 @@
         <v>219</v>
       </c>
       <c r="L3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="64.8" customHeight="1">
@@ -4721,7 +4725,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F1" t="s">
         <v>222</v>
@@ -4730,7 +4734,7 @@
         <v>223</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4754,7 +4758,7 @@
         <v>320</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="H4" s="29"/>
     </row>
@@ -4811,7 +4815,7 @@
         <v>232</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4826,21 +4830,21 @@
         <v>235</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="F11" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add usable to vaccine carriers
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="533">
   <si>
     <t>clause</t>
   </si>
@@ -1035,18 +1035,6 @@
     <t>(kilómetros)</t>
   </si>
   <si>
-    <t>Total number of vaccine carriers at facility</t>
-  </si>
-  <si>
-    <t>Número total de portadores de vacunas en la facilidad</t>
-  </si>
-  <si>
-    <t>Total number of vaccine carriers at facility?</t>
-  </si>
-  <si>
-    <t>Número total de portadores de vacunas en la facilidad?</t>
-  </si>
-  <si>
     <t>display.title.text.fr</t>
   </si>
   <si>
@@ -1245,9 +1233,6 @@
     <t>Numéro de téléphone de la personne à contacter</t>
   </si>
   <si>
-    <t>Nombre de porte-vaccins dans l'établissement</t>
-  </si>
-  <si>
     <t>Nombre de glacières pour congélation sûre dans l'établissement</t>
   </si>
   <si>
@@ -1621,6 +1606,24 @@
   </si>
   <si>
     <t>Nombre total de glacières utilisables dans l'installation?</t>
+  </si>
+  <si>
+    <t>Total number of usable vaccine carriers at facility</t>
+  </si>
+  <si>
+    <t>Número total de portadores de vacunas utilizables en la facilidad</t>
+  </si>
+  <si>
+    <t>Nombre total de porte-vaccins utilisables dans l'établissement</t>
+  </si>
+  <si>
+    <t>Total number of usable vaccine carriers at facility?</t>
+  </si>
+  <si>
+    <t>Número total de portadores de vacunas utilizables en la facilidad?</t>
+  </si>
+  <si>
+    <t>Nombre total de porte-vaccins utilisables dans l'établissement?</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1747,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1820,6 +1823,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2256,27 +2266,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="78">
       <c r="A3" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2289,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K35" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -2330,7 +2340,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -2339,7 +2349,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>332</v>
@@ -2348,7 +2358,7 @@
         <v>333</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>9</v>
@@ -2357,16 +2367,16 @@
         <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="29" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2380,7 +2390,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="29" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2417,7 +2427,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -2426,7 +2436,7 @@
         <v>15</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2451,7 +2461,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I5" t="s">
         <v>20</v>
@@ -2460,7 +2470,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="P5" t="b">
         <f>TRUE()</f>
@@ -2495,7 +2505,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I8" t="s">
         <v>25</v>
@@ -2504,7 +2514,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="33" customFormat="1">
@@ -2515,27 +2525,27 @@
         <v>55</v>
       </c>
       <c r="E9" s="33" t="s">
+        <v>472</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>474</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>475</v>
+      </c>
+      <c r="I9" s="33" t="s">
         <v>477</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>479</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>480</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>482</v>
-      </c>
       <c r="J9" s="33" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="29" customFormat="1">
       <c r="A10" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>478</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>483</v>
       </c>
       <c r="H10" s="30"/>
       <c r="K10" s="30"/>
@@ -2557,7 +2567,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I11" t="s">
         <v>27</v>
@@ -2566,7 +2576,7 @@
         <v>28</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="P11">
         <v>1</v>
@@ -2610,7 +2620,7 @@
         <v>33</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I15" t="s">
         <v>34</v>
@@ -2619,7 +2629,7 @@
         <v>33</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2639,7 +2649,7 @@
         <v>38</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I16" t="s">
         <v>39</v>
@@ -2648,7 +2658,7 @@
         <v>38</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -2665,7 +2675,7 @@
         <v>288</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I17" t="s">
         <v>289</v>
@@ -2674,7 +2684,7 @@
         <v>288</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -2708,7 +2718,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
@@ -2717,7 +2727,7 @@
         <v>45</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -2725,7 +2735,7 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="H21" s="17"/>
       <c r="K21" s="22"/>
@@ -2747,7 +2757,7 @@
         <v>51</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I22" s="33" t="s">
         <v>52</v>
@@ -2756,13 +2766,13 @@
         <v>51</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="L22" s="33" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="M22" s="33" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2783,22 +2793,22 @@
         <v>54</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2829,7 +2839,7 @@
         <v>59</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="I27" s="33" t="s">
         <v>60</v>
@@ -2838,7 +2848,7 @@
         <v>298</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="L27" s="33" t="s">
         <v>334</v>
@@ -2864,7 +2874,7 @@
         <v>62</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I28" t="s">
         <v>63</v>
@@ -2873,7 +2883,7 @@
         <v>294</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2904,7 +2914,7 @@
         <v>66</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I31" t="s">
         <v>293</v>
@@ -2913,7 +2923,7 @@
         <v>295</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2933,7 +2943,7 @@
         <v>70</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I32" t="s">
         <v>71</v>
@@ -2942,7 +2952,7 @@
         <v>296</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2973,7 +2983,7 @@
         <v>74</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I35" t="s">
         <v>75</v>
@@ -2982,7 +2992,7 @@
         <v>297</v>
       </c>
       <c r="K35" s="25" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="31.2">
@@ -2999,7 +3009,7 @@
         <v>275</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I36" t="s">
         <v>276</v>
@@ -3008,7 +3018,7 @@
         <v>277</v>
       </c>
       <c r="K36" s="25" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
@@ -3028,16 +3038,16 @@
         <v>278</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I37" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="J37" s="11" t="s">
         <v>279</v>
       </c>
       <c r="K37" s="25" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
@@ -3060,19 +3070,19 @@
         <v>40</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="35" customFormat="1" ht="19.05" customHeight="1">
@@ -3080,19 +3090,19 @@
         <v>40</v>
       </c>
       <c r="E41" s="35" t="s">
+        <v>501</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>503</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>504</v>
+      </c>
+      <c r="I41" s="35" t="s">
+        <v>505</v>
+      </c>
+      <c r="J41" s="35" t="s">
         <v>506</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>508</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>509</v>
-      </c>
-      <c r="I41" s="35" t="s">
-        <v>510</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="30" customFormat="1">
@@ -3117,22 +3127,22 @@
         <v>271</v>
       </c>
       <c r="F44" s="33" t="s">
+        <v>521</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>522</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>523</v>
+      </c>
+      <c r="I44" s="33" t="s">
+        <v>524</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>525</v>
+      </c>
+      <c r="K44" s="34" t="s">
         <v>526</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>527</v>
-      </c>
-      <c r="H44" s="34" t="s">
-        <v>528</v>
-      </c>
-      <c r="I44" s="33" t="s">
-        <v>529</v>
-      </c>
-      <c r="J44" s="36" t="s">
-        <v>530</v>
-      </c>
-      <c r="K44" s="34" t="s">
-        <v>531</v>
       </c>
       <c r="L44" s="36"/>
       <c r="M44" s="36"/>
@@ -3152,7 +3162,7 @@
         <v>282</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>280</v>
@@ -3161,7 +3171,7 @@
         <v>283</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
@@ -3183,34 +3193,34 @@
       <c r="H47" s="17"/>
       <c r="K47" s="22"/>
     </row>
-    <row r="48" spans="1:14" ht="29.4" thickBot="1">
-      <c r="C48" t="s">
+    <row r="48" spans="1:14" s="33" customFormat="1" ht="29.4" thickBot="1">
+      <c r="C48" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="H48" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="K48" s="26" t="s">
-        <v>406</v>
-      </c>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
+      <c r="F48" s="37" t="s">
+        <v>527</v>
+      </c>
+      <c r="G48" s="38" t="s">
+        <v>528</v>
+      </c>
+      <c r="H48" s="39" t="s">
+        <v>529</v>
+      </c>
+      <c r="I48" s="37" t="s">
+        <v>530</v>
+      </c>
+      <c r="J48" s="38" t="s">
+        <v>531</v>
+      </c>
+      <c r="K48" s="39" t="s">
+        <v>532</v>
+      </c>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
     </row>
     <row r="49" spans="1:14" ht="43.8" thickBot="1">
       <c r="C49" t="s">
@@ -3226,7 +3236,7 @@
         <v>284</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="I49" s="9" t="s">
         <v>281</v>
@@ -3235,7 +3245,7 @@
         <v>285</v>
       </c>
       <c r="K49" s="26" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
@@ -3258,19 +3268,19 @@
         <v>40</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="G52" s="33" t="s">
+        <v>490</v>
+      </c>
+      <c r="I52" s="33" t="s">
         <v>495</v>
       </c>
-      <c r="I52" s="33" t="s">
-        <v>500</v>
-      </c>
       <c r="J52" s="33" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="33" customFormat="1">
@@ -3278,19 +3288,19 @@
         <v>40</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="I53" s="33" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="J53" s="33" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:14" s="33" customFormat="1">
@@ -3298,19 +3308,19 @@
         <v>40</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="F54" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="I54" s="33" t="s">
         <v>498</v>
       </c>
-      <c r="G54" s="33" t="s">
-        <v>499</v>
-      </c>
-      <c r="I54" s="33" t="s">
-        <v>503</v>
-      </c>
       <c r="J54" s="33" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3346,7 +3356,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3354,7 +3364,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C2" s="29" t="b">
         <v>1</v>
@@ -3365,7 +3375,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3373,7 +3383,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3381,7 +3391,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3421,7 +3431,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3438,7 +3448,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3455,7 +3465,7 @@
         <v>82</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3472,7 +3482,7 @@
         <v>85</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3489,7 +3499,7 @@
         <v>88</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3506,7 +3516,7 @@
         <v>91</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3523,7 +3533,7 @@
         <v>94</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3540,7 +3550,7 @@
         <v>97</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3557,7 +3567,7 @@
         <v>100</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3574,7 +3584,7 @@
         <v>103</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3591,7 +3601,7 @@
         <v>106</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3608,7 +3618,7 @@
         <v>109</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17.100000000000001" customHeight="1">
@@ -3625,7 +3635,7 @@
         <v>112</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3642,7 +3652,7 @@
         <v>301</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1">
@@ -3659,7 +3669,7 @@
         <v>115</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3676,7 +3686,7 @@
         <v>118</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3698,13 +3708,13 @@
         <v>30</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="29" customFormat="1">
@@ -3712,13 +3722,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="29" customFormat="1">
@@ -3726,13 +3736,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="29" customFormat="1">
@@ -3740,13 +3750,13 @@
         <v>30</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="29" customFormat="1">
@@ -3754,13 +3764,13 @@
         <v>30</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="29" customFormat="1">
@@ -3768,13 +3778,13 @@
         <v>30</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="29" customFormat="1">
@@ -3782,13 +3792,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="29" customFormat="1">
@@ -3796,13 +3806,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="29" customFormat="1">
@@ -3810,13 +3820,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="29" customFormat="1">
@@ -3824,13 +3834,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="29" customFormat="1">
@@ -3838,13 +3848,13 @@
         <v>30</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="29" customFormat="1">
@@ -3852,13 +3862,13 @@
         <v>30</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="29" customFormat="1">
@@ -3866,13 +3876,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="29" customFormat="1">
@@ -3880,10 +3890,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="29" customFormat="1"/>
@@ -3918,7 +3928,7 @@
         <v>124</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3952,7 +3962,7 @@
         <v>130</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3969,7 +3979,7 @@
         <v>133</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3986,7 +3996,7 @@
         <v>135</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -4003,7 +4013,7 @@
         <v>303</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4020,7 +4030,7 @@
         <v>138</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -4037,7 +4047,7 @@
         <v>141</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -4054,7 +4064,7 @@
         <v>308</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="31.2">
@@ -4071,7 +4081,7 @@
         <v>316</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="33" customFormat="1">
@@ -4079,13 +4089,13 @@
         <v>42</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D46" s="33" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E46" s="34"/>
     </row>
@@ -4103,7 +4113,7 @@
         <v>144</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4120,7 +4130,7 @@
         <v>147</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -4137,7 +4147,7 @@
         <v>150</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -4154,7 +4164,7 @@
         <v>153</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -4171,7 +4181,7 @@
         <v>156</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -4188,7 +4198,7 @@
         <v>157</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4222,7 +4232,7 @@
         <v>162</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -4239,7 +4249,7 @@
         <v>165</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -4256,7 +4266,7 @@
         <v>168</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -4273,7 +4283,7 @@
         <v>171</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4290,7 +4300,7 @@
         <v>173</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4307,7 +4317,7 @@
         <v>176</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -4324,7 +4334,7 @@
         <v>179</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -4341,7 +4351,7 @@
         <v>182</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -4358,7 +4368,7 @@
         <v>185</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -4375,7 +4385,7 @@
         <v>187</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -4392,7 +4402,7 @@
         <v>314</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -4409,7 +4419,7 @@
         <v>191</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -4426,7 +4436,7 @@
         <v>193</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4443,7 +4453,7 @@
         <v>313</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -4460,7 +4470,7 @@
         <v>144</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4477,7 +4487,7 @@
         <v>196</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4494,7 +4504,7 @@
         <v>199</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4511,7 +4521,7 @@
         <v>201</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4528,7 +4538,7 @@
         <v>157</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4545,7 +4555,7 @@
         <v>168</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -4613,7 +4623,7 @@
         <v>212</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="26.1" customHeight="1">
@@ -4674,7 +4684,7 @@
         <v>219</v>
       </c>
       <c r="L3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="64.8" customHeight="1">
@@ -4725,7 +4735,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F1" t="s">
         <v>222</v>
@@ -4734,7 +4744,7 @@
         <v>223</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4758,7 +4768,7 @@
         <v>320</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="H4" s="29"/>
     </row>
@@ -4815,7 +4825,7 @@
         <v>232</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4830,21 +4840,21 @@
         <v>235</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="F11" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hide freeze safe questions
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="534">
   <si>
     <t>clause</t>
   </si>
@@ -1624,6 +1624,9 @@
   </si>
   <si>
     <t>Nombre total de porte-vaccins utilisables dans l'établissement?</t>
+  </si>
+  <si>
+    <t>(false)</t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1750,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1829,6 +1832,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2297,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -3119,7 +3128,7 @@
       <c r="H43" s="17"/>
       <c r="K43" s="22"/>
     </row>
-    <row r="44" spans="1:14" s="33" customFormat="1" ht="31.8" thickBot="1">
+    <row r="44" spans="1:14" s="33" customFormat="1" ht="31.2">
       <c r="C44" s="33" t="s">
         <v>40</v>
       </c>
@@ -3148,183 +3157,243 @@
       <c r="M44" s="36"/>
       <c r="N44" s="36"/>
     </row>
-    <row r="45" spans="1:14" ht="43.8" thickBot="1">
-      <c r="C45" t="s">
+    <row r="45" spans="1:14" s="30" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A45" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>533</v>
+      </c>
+      <c r="G45" s="41"/>
+      <c r="H45" s="25"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+    </row>
+    <row r="46" spans="1:14" ht="43.8" thickBot="1">
+      <c r="C46" t="s">
         <v>40</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>273</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F46" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G46" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="H46" s="21" t="s">
         <v>402</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="I46" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="J45" s="12" t="s">
+      <c r="J46" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="K45" s="26" t="s">
+      <c r="K46" s="26" t="s">
         <v>402</v>
       </c>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-    </row>
-    <row r="46" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A46" t="s">
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" s="29" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A47" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="H46" s="17"/>
-      <c r="K46" s="22"/>
-    </row>
-    <row r="47" spans="1:14" ht="16.2" thickBot="1">
-      <c r="A47" t="s">
+      <c r="F48" s="9"/>
+      <c r="H48" s="17"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A49" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="9"/>
-      <c r="H47" s="17"/>
-      <c r="K47" s="22"/>
-    </row>
-    <row r="48" spans="1:14" s="33" customFormat="1" ht="29.4" thickBot="1">
-      <c r="C48" s="33" t="s">
+      <c r="F49" s="9"/>
+      <c r="H49" s="17"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" spans="1:14" s="33" customFormat="1" ht="29.4" thickBot="1">
+      <c r="C50" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E50" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F50" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="G48" s="38" t="s">
+      <c r="G50" s="38" t="s">
         <v>528</v>
       </c>
-      <c r="H48" s="39" t="s">
+      <c r="H50" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="I48" s="37" t="s">
+      <c r="I50" s="37" t="s">
         <v>530</v>
       </c>
-      <c r="J48" s="38" t="s">
+      <c r="J50" s="38" t="s">
         <v>531</v>
       </c>
-      <c r="K48" s="39" t="s">
+      <c r="K50" s="39" t="s">
         <v>532</v>
       </c>
-      <c r="L48" s="38"/>
-      <c r="M48" s="38"/>
-      <c r="N48" s="38"/>
-    </row>
-    <row r="49" spans="1:14" ht="43.8" thickBot="1">
-      <c r="C49" t="s">
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+    </row>
+    <row r="51" spans="1:14" s="30" customFormat="1" ht="16.2" thickBot="1">
+      <c r="A51" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>533</v>
+      </c>
+      <c r="F51" s="42"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
+      <c r="N51" s="43"/>
+    </row>
+    <row r="52" spans="1:14" ht="43.8" thickBot="1">
+      <c r="C52" t="s">
         <v>40</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>274</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F52" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="G49" s="12" t="s">
+      <c r="G52" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>403</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="I52" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="J52" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="K49" s="26" t="s">
+      <c r="K52" s="26" t="s">
         <v>403</v>
       </c>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-    </row>
-    <row r="50" spans="1:14">
-      <c r="A50" t="s">
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+    </row>
+    <row r="53" spans="1:14" s="29" customFormat="1">
+      <c r="A53" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" s="40"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="40"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
         <v>21</v>
       </c>
-      <c r="H50" s="17"/>
-      <c r="K50" s="22"/>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="33" customFormat="1">
-      <c r="C52" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E52" s="33" t="s">
-        <v>486</v>
-      </c>
-      <c r="F52" s="33" t="s">
-        <v>488</v>
-      </c>
-      <c r="G52" s="33" t="s">
-        <v>490</v>
-      </c>
-      <c r="I52" s="33" t="s">
-        <v>495</v>
-      </c>
-      <c r="J52" s="33" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" s="33" customFormat="1">
-      <c r="C53" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="33" t="s">
-        <v>487</v>
-      </c>
-      <c r="F53" s="33" t="s">
-        <v>489</v>
-      </c>
-      <c r="G53" s="33" t="s">
-        <v>491</v>
-      </c>
-      <c r="I53" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="J53" s="33" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" s="33" customFormat="1">
-      <c r="C54" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E54" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="F54" s="33" t="s">
-        <v>493</v>
-      </c>
-      <c r="G54" s="33" t="s">
-        <v>494</v>
-      </c>
-      <c r="I54" s="33" t="s">
-        <v>498</v>
-      </c>
-      <c r="J54" s="33" t="s">
-        <v>500</v>
-      </c>
+      <c r="H54" s="17"/>
+      <c r="K54" s="22"/>
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" s="33" customFormat="1">
+      <c r="C56" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>486</v>
+      </c>
+      <c r="F56" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>490</v>
+      </c>
+      <c r="I56" s="33" t="s">
+        <v>495</v>
+      </c>
+      <c r="J56" s="33" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" s="33" customFormat="1">
+      <c r="C57" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="F57" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="G57" s="33" t="s">
+        <v>491</v>
+      </c>
+      <c r="I57" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="J57" s="33" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" s="33" customFormat="1">
+      <c r="C58" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="F58" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="I58" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="J58" s="33" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add usable to number of 0.x liter ice packs
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
+++ b/app/config/tables/health_facilities/forms/health_facilities/health_facilities.xlsx
@@ -1491,45 +1491,9 @@
     <t>number_of_l4_packs</t>
   </si>
   <si>
-    <t>Number of 0.3 liter ice/water packs</t>
-  </si>
-  <si>
-    <t>Number of 0.4 liter ice/water packs</t>
-  </si>
-  <si>
-    <t>Número de paquetes de hielo/agua de 0.3 litros</t>
-  </si>
-  <si>
-    <t>Número de paquetes de hielo/agua de 0.4 litros</t>
-  </si>
-  <si>
     <t>number_of_l6_packs</t>
   </si>
   <si>
-    <t>Number of 0.6 liter ice/water packs</t>
-  </si>
-  <si>
-    <t>Número de paquetes de hielo/agua de 0.6 litros</t>
-  </si>
-  <si>
-    <t>Total number of 0.3 liter ice/water packs?</t>
-  </si>
-  <si>
-    <t>Número total de paquetes de hielo/agua de 0.3 litros?</t>
-  </si>
-  <si>
-    <t>Total number of 0.4 liter ice/water packs?</t>
-  </si>
-  <si>
-    <t>Total number of 0.6 liter ice/water packs?</t>
-  </si>
-  <si>
-    <t>Número total de paquetes de hielo/agua de 0.4 litros?</t>
-  </si>
-  <si>
-    <t>Número total de paquetes de hielo/agua de 0.6 litros?</t>
-  </si>
-  <si>
     <t>spare_temp_monitoring_devices</t>
   </si>
   <si>
@@ -1627,6 +1591,42 @@
   </si>
   <si>
     <t>(false)</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.3 litros utilizables</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.4 litros utilizables</t>
+  </si>
+  <si>
+    <t>Número de paquetes de hielo/agua de 0.6 litros utilizables</t>
+  </si>
+  <si>
+    <t>Number of usable 0.3 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Number of usable 0.4 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Number of usable 0.6 liter ice/water packs</t>
+  </si>
+  <si>
+    <t>Total number of usable 0.3 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Total number of usable 0.4 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Total number of usable 0.6 liter ice/water packs?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.3 litros utilizables?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.4 litros utilizables?</t>
+  </si>
+  <si>
+    <t>Número total de paquetes de hielo/agua de 0.6 litros utilizables?</t>
   </si>
 </sst>
 </file>
@@ -2308,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="J47" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -2319,7 +2319,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.296875" customWidth="1"/>
     <col min="5" max="5" width="35.59765625" customWidth="1"/>
-    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="43.19921875" customWidth="1"/>
     <col min="7" max="7" width="33.796875" customWidth="1"/>
     <col min="8" max="9" width="26.796875" customWidth="1"/>
     <col min="10" max="15" width="47.59765625" customWidth="1"/>
@@ -2376,16 +2376,16 @@
         <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="29" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2399,7 +2399,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="29" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2802,22 +2802,22 @@
         <v>54</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3079,19 +3079,19 @@
         <v>40</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="35" customFormat="1" ht="19.05" customHeight="1">
@@ -3099,19 +3099,19 @@
         <v>40</v>
       </c>
       <c r="E41" s="35" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="I41" s="35" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="J41" s="35" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="30" customFormat="1">
@@ -3136,22 +3136,22 @@
         <v>271</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="G44" s="36" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="I44" s="33" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="J44" s="36" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="L44" s="36"/>
       <c r="M44" s="36"/>
@@ -3162,7 +3162,7 @@
         <v>47</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="G45" s="41"/>
       <c r="H45" s="25"/>
@@ -3239,22 +3239,22 @@
         <v>272</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="G50" s="38" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="H50" s="39" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="I50" s="37" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="J50" s="38" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="K50" s="39" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
@@ -3265,7 +3265,7 @@
         <v>47</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="F51" s="42"/>
       <c r="G51" s="43"/>
@@ -3340,16 +3340,16 @@
         <v>486</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>488</v>
+        <v>525</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>490</v>
+        <v>522</v>
       </c>
       <c r="I56" s="33" t="s">
-        <v>495</v>
+        <v>528</v>
       </c>
       <c r="J56" s="33" t="s">
-        <v>496</v>
+        <v>531</v>
       </c>
     </row>
     <row r="57" spans="1:14" s="33" customFormat="1">
@@ -3360,16 +3360,16 @@
         <v>487</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>489</v>
+        <v>526</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>491</v>
+        <v>523</v>
       </c>
       <c r="I57" s="33" t="s">
-        <v>497</v>
+        <v>529</v>
       </c>
       <c r="J57" s="33" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
     </row>
     <row r="58" spans="1:14" s="33" customFormat="1">
@@ -3377,19 +3377,19 @@
         <v>40</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>493</v>
+        <v>527</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="I58" s="33" t="s">
-        <v>498</v>
+        <v>530</v>
       </c>
       <c r="J58" s="33" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3444,7 +3444,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3452,7 +3452,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3460,7 +3460,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>